<commit_message>
remote cost&weight & fixed reward
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.364</v>
+        <v>0.364</v>
       </c>
       <c r="B1" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.044</v>
       </c>
       <c r="C1" t="n">
-        <v>0.444</v>
+        <v>-0.335</v>
       </c>
       <c r="D1" t="n">
-        <v>159</v>
+        <v>-122</v>
       </c>
       <c r="E1" t="n">
-        <v>-31</v>
+        <v>47</v>
       </c>
       <c r="F1" t="n">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.508</v>
+        <v>0.051</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.046</v>
+        <v>0.11</v>
       </c>
       <c r="C2" t="n">
-        <v>0.049</v>
+        <v>-0.096</v>
       </c>
       <c r="D2" t="n">
-        <v>121</v>
+        <v>-63</v>
       </c>
       <c r="E2" t="n">
-        <v>-19</v>
+        <v>17</v>
       </c>
       <c r="F2" t="n">
-        <v>172</v>
+        <v>-98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.049</v>
+        <v>-0.3</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.332</v>
+        <v>-0.097</v>
       </c>
       <c r="C3" t="n">
-        <v>0.394</v>
+        <v>-0.61</v>
       </c>
       <c r="D3" t="n">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="E3" t="n">
-        <v>-46</v>
+        <v>-59</v>
       </c>
       <c r="F3" t="n">
-        <v>129</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.096</v>
+        <v>0.116</v>
       </c>
       <c r="B4" t="n">
-        <v>0.08799999999999999</v>
+        <v>-0.024</v>
       </c>
       <c r="C4" t="n">
-        <v>0.097</v>
+        <v>0.543</v>
       </c>
       <c r="D4" t="n">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
-        <v>-46</v>
+        <v>-37</v>
       </c>
       <c r="F4" t="n">
-        <v>-40</v>
+        <v>-164</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.152</v>
+        <v>0.017</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.211</v>
+        <v>0.571</v>
       </c>
       <c r="C5" t="n">
-        <v>0.342</v>
+        <v>-0.282</v>
       </c>
       <c r="D5" t="n">
-        <v>28</v>
+        <v>-28</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-160</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.038</v>
+        <v>-0.396</v>
       </c>
       <c r="B6" t="n">
-        <v>0.151</v>
+        <v>0.258</v>
       </c>
       <c r="C6" t="n">
-        <v>0.369</v>
+        <v>0.663</v>
       </c>
       <c r="D6" t="n">
-        <v>-126</v>
+        <v>-1</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>-45</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.324</v>
+        <v>0.196</v>
       </c>
       <c r="B7" t="n">
-        <v>0.034</v>
+        <v>-0.074</v>
       </c>
       <c r="C7" t="n">
-        <v>0.017</v>
+        <v>-0.369</v>
       </c>
       <c r="D7" t="n">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="E7" t="n">
-        <v>-54</v>
+        <v>40</v>
       </c>
       <c r="F7" t="n">
-        <v>36</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.007</v>
+        <v>0.026</v>
       </c>
       <c r="B8" t="n">
-        <v>0.171</v>
+        <v>-0.197</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.146</v>
+        <v>-0.142</v>
       </c>
       <c r="D8" t="n">
-        <v>-59</v>
+        <v>84</v>
       </c>
       <c r="E8" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F8" t="n">
-        <v>-21</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.024</v>
+        <v>0.498</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.183</v>
+        <v>-0.305</v>
       </c>
       <c r="C9" t="n">
-        <v>0.225</v>
+        <v>0.572</v>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>-16</v>
       </c>
       <c r="F9" t="n">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.047</v>
+        <v>0.08</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.203</v>
+        <v>-0.082</v>
       </c>
       <c r="C10" t="n">
-        <v>0.116</v>
+        <v>0.051</v>
       </c>
       <c r="D10" t="n">
-        <v>-48</v>
+        <v>17</v>
       </c>
       <c r="E10" t="n">
         <v>57</v>
       </c>
       <c r="F10" t="n">
-        <v>-65</v>
+        <v>-88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 4,5,6 dof robot model
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.364</v>
+        <v>0.119</v>
       </c>
       <c r="B1" t="n">
-        <v>0.044</v>
+        <v>-0.401</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.335</v>
+        <v>0.264</v>
       </c>
       <c r="D1" t="n">
-        <v>-122</v>
+        <v>-74</v>
       </c>
       <c r="E1" t="n">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F1" t="n">
-        <v>101</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.051</v>
+        <v>0.001</v>
       </c>
       <c r="B2" t="n">
-        <v>0.11</v>
+        <v>0.124</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.096</v>
+        <v>-0.064</v>
       </c>
       <c r="D2" t="n">
-        <v>-63</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>17</v>
+        <v>-68</v>
       </c>
       <c r="F2" t="n">
-        <v>-98</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.3</v>
+        <v>0.019</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.097</v>
+        <v>-0.297</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.61</v>
+        <v>0.887</v>
       </c>
       <c r="D3" t="n">
-        <v>157</v>
+        <v>90</v>
       </c>
       <c r="E3" t="n">
-        <v>-59</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
-        <v>-8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.116</v>
+        <v>-0.022</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.024</v>
+        <v>-0.819</v>
       </c>
       <c r="C4" t="n">
-        <v>0.543</v>
+        <v>0.211</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="E4" t="n">
-        <v>-37</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>-164</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.017</v>
+        <v>-0.162</v>
       </c>
       <c r="B5" t="n">
-        <v>0.571</v>
+        <v>-0.26</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.282</v>
+        <v>-0.289</v>
       </c>
       <c r="D5" t="n">
-        <v>-28</v>
+        <v>97</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F5" t="n">
-        <v>-90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.396</v>
+        <v>-0.082</v>
       </c>
       <c r="B6" t="n">
-        <v>0.258</v>
+        <v>-0.134</v>
       </c>
       <c r="C6" t="n">
-        <v>0.663</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>-1</v>
+        <v>-116</v>
       </c>
       <c r="E6" t="n">
-        <v>-45</v>
+        <v>57</v>
       </c>
       <c r="F6" t="n">
-        <v>176</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.196</v>
+        <v>-0.062</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.074</v>
+        <v>-0.043</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.369</v>
+        <v>0.18</v>
       </c>
       <c r="D7" t="n">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>-61</v>
       </c>
       <c r="F7" t="n">
-        <v>135</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.026</v>
+        <v>-0.156</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.197</v>
+        <v>0.037</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.142</v>
+        <v>-0.007</v>
       </c>
       <c r="D8" t="n">
-        <v>84</v>
+        <v>-79</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>-39</v>
       </c>
       <c r="F8" t="n">
-        <v>-33</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.498</v>
+        <v>0.49</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.305</v>
+        <v>-0.112</v>
       </c>
       <c r="C9" t="n">
-        <v>0.572</v>
+        <v>-0.262</v>
       </c>
       <c r="D9" t="n">
-        <v>76</v>
+        <v>-22</v>
       </c>
       <c r="E9" t="n">
-        <v>-16</v>
+        <v>-11</v>
       </c>
       <c r="F9" t="n">
-        <v>62</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.08</v>
+        <v>0.31</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.082</v>
+        <v>0.192</v>
       </c>
       <c r="C10" t="n">
-        <v>0.051</v>
+        <v>0.083</v>
       </c>
       <c r="D10" t="n">
-        <v>17</v>
+        <v>-85</v>
       </c>
       <c r="E10" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F10" t="n">
-        <v>-88</v>
+        <v>-116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed reach_manipulability_evaluate  count = 0
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.119</v>
+        <v>-0.041</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.401</v>
+        <v>0.149</v>
       </c>
       <c r="C1" t="n">
-        <v>0.264</v>
+        <v>-0.04</v>
       </c>
       <c r="D1" t="n">
-        <v>-74</v>
+        <v>-49</v>
       </c>
       <c r="E1" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="F1" t="n">
-        <v>-34</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.001</v>
+        <v>-0.426</v>
       </c>
       <c r="B2" t="n">
-        <v>0.124</v>
+        <v>-0.471</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.064</v>
+        <v>0.553</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>-93</v>
       </c>
       <c r="E2" t="n">
-        <v>-68</v>
+        <v>-10</v>
       </c>
       <c r="F2" t="n">
-        <v>-13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.019</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.297</v>
+        <v>-0.613</v>
       </c>
       <c r="C3" t="n">
-        <v>0.887</v>
+        <v>0.133</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>-78</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>-45</v>
       </c>
       <c r="F3" t="n">
-        <v>58</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.022</v>
+        <v>-0.038</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.819</v>
+        <v>0.16</v>
       </c>
       <c r="C4" t="n">
-        <v>0.211</v>
+        <v>0.174</v>
       </c>
       <c r="D4" t="n">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>-12</v>
       </c>
       <c r="F4" t="n">
-        <v>134</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.162</v>
+        <v>0.113</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.26</v>
+        <v>-0.127</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.289</v>
+        <v>-0.016</v>
       </c>
       <c r="D5" t="n">
-        <v>97</v>
+        <v>-63</v>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>-1</v>
       </c>
       <c r="F5" t="n">
-        <v>61</v>
+        <v>-154</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.082</v>
+        <v>0.424</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.134</v>
+        <v>-0.042</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6899999999999999</v>
+        <v>-0.271</v>
       </c>
       <c r="D6" t="n">
-        <v>-116</v>
+        <v>-141</v>
       </c>
       <c r="E6" t="n">
         <v>57</v>
       </c>
       <c r="F6" t="n">
-        <v>-74</v>
+        <v>-109</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.062</v>
+        <v>0.336</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.043</v>
+        <v>-0.375</v>
       </c>
       <c r="C7" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="D7" t="n">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="E7" t="n">
-        <v>-61</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>153</v>
+        <v>-108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.156</v>
+        <v>0.129</v>
       </c>
       <c r="B8" t="n">
-        <v>0.037</v>
+        <v>-0.434</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.007</v>
+        <v>0.5</v>
       </c>
       <c r="D8" t="n">
-        <v>-79</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>-39</v>
+        <v>-17</v>
       </c>
       <c r="F8" t="n">
-        <v>173</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.49</v>
+        <v>-0.217</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.112</v>
+        <v>-0.165</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.262</v>
+        <v>0.09</v>
       </c>
       <c r="D9" t="n">
-        <v>-22</v>
+        <v>-128</v>
       </c>
       <c r="E9" t="n">
-        <v>-11</v>
+        <v>57</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>-177</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.31</v>
+        <v>0.135</v>
       </c>
       <c r="B10" t="n">
-        <v>0.192</v>
+        <v>-0.136</v>
       </c>
       <c r="C10" t="n">
-        <v>0.083</v>
+        <v>0.451</v>
       </c>
       <c r="D10" t="n">
-        <v>-85</v>
+        <v>-73</v>
       </c>
       <c r="E10" t="n">
-        <v>29</v>
+        <v>-16</v>
       </c>
       <c r="F10" t="n">
-        <v>-116</v>
+        <v>-104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
design reward function version1
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,182 +423,182 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.041</v>
+        <v>-0.424</v>
       </c>
       <c r="B1" t="n">
-        <v>0.149</v>
+        <v>-0.051</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.04</v>
+        <v>0.845</v>
       </c>
       <c r="D1" t="n">
-        <v>-49</v>
+        <v>27</v>
       </c>
       <c r="E1" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="F1" t="n">
-        <v>-25</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.426</v>
+        <v>-0.075</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.471</v>
+        <v>-0.291</v>
       </c>
       <c r="C2" t="n">
-        <v>0.553</v>
+        <v>0.656</v>
       </c>
       <c r="D2" t="n">
-        <v>-93</v>
+        <v>-123</v>
       </c>
       <c r="E2" t="n">
-        <v>-10</v>
+        <v>47</v>
       </c>
       <c r="F2" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.263</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.613</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.133</v>
+        <v>0.35</v>
       </c>
       <c r="D3" t="n">
-        <v>-78</v>
+        <v>-15</v>
       </c>
       <c r="E3" t="n">
-        <v>-45</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>-105</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.038</v>
+        <v>0.138</v>
       </c>
       <c r="B4" t="n">
-        <v>0.16</v>
+        <v>0.179</v>
       </c>
       <c r="C4" t="n">
-        <v>0.174</v>
+        <v>0.991</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="E4" t="n">
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="F4" t="n">
-        <v>-23</v>
+        <v>-121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.113</v>
+        <v>0.231</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.127</v>
+        <v>0.01</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.016</v>
+        <v>0.795</v>
       </c>
       <c r="D5" t="n">
-        <v>-63</v>
+        <v>67</v>
       </c>
       <c r="E5" t="n">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="F5" t="n">
-        <v>-154</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.424</v>
+        <v>-0.227</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.042</v>
+        <v>-0.309</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.271</v>
+        <v>-0.508</v>
       </c>
       <c r="D6" t="n">
-        <v>-141</v>
+        <v>124</v>
       </c>
       <c r="E6" t="n">
-        <v>57</v>
+        <v>-2</v>
       </c>
       <c r="F6" t="n">
-        <v>-109</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.336</v>
+        <v>0.519</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.375</v>
+        <v>-0.447</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09</v>
+        <v>0.052</v>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
-        <v>-108</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.129</v>
+        <v>-0.273</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.434</v>
+        <v>-0.369</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D8" t="n">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="E8" t="n">
-        <v>-17</v>
+        <v>25</v>
       </c>
       <c r="F8" t="n">
-        <v>-63</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.217</v>
+        <v>0.001</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.165</v>
+        <v>-0.118</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09</v>
+        <v>-0.12</v>
       </c>
       <c r="D9" t="n">
-        <v>-128</v>
+        <v>177</v>
       </c>
       <c r="E9" t="n">
-        <v>57</v>
+        <v>-29</v>
       </c>
       <c r="F9" t="n">
-        <v>-177</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="10">
@@ -606,19 +606,19 @@
         <v>0.135</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.136</v>
+        <v>-0.238</v>
       </c>
       <c r="C10" t="n">
-        <v>0.451</v>
+        <v>-0.501</v>
       </c>
       <c r="D10" t="n">
-        <v>-73</v>
+        <v>-84</v>
       </c>
       <c r="E10" t="n">
-        <v>-16</v>
+        <v>-11</v>
       </c>
       <c r="F10" t="n">
-        <v>-104</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test model select input
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.424</v>
+        <v>0.382</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.051</v>
+        <v>0.537</v>
       </c>
       <c r="C1" t="n">
-        <v>0.845</v>
+        <v>-0.121</v>
       </c>
       <c r="D1" t="n">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="E1" t="n">
-        <v>60</v>
+        <v>-34</v>
       </c>
       <c r="F1" t="n">
-        <v>-58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.075</v>
+        <v>-0.508</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.291</v>
+        <v>-0.249</v>
       </c>
       <c r="C2" t="n">
-        <v>0.656</v>
+        <v>0.233</v>
       </c>
       <c r="D2" t="n">
-        <v>-123</v>
+        <v>141</v>
       </c>
       <c r="E2" t="n">
-        <v>47</v>
+        <v>-10</v>
       </c>
       <c r="F2" t="n">
-        <v>29</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.263</v>
+        <v>0.095</v>
       </c>
       <c r="B3" t="n">
-        <v>0.08500000000000001</v>
+        <v>-0.262</v>
       </c>
       <c r="C3" t="n">
-        <v>0.35</v>
+        <v>-0.276</v>
       </c>
       <c r="D3" t="n">
-        <v>-15</v>
+        <v>-148</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>-79</v>
       </c>
       <c r="F3" t="n">
-        <v>70</v>
+        <v>-67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.138</v>
+        <v>-0.596</v>
       </c>
       <c r="B4" t="n">
-        <v>0.179</v>
+        <v>-0.473</v>
       </c>
       <c r="C4" t="n">
-        <v>0.991</v>
+        <v>-0.035</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E4" t="n">
-        <v>-15</v>
+        <v>-27</v>
       </c>
       <c r="F4" t="n">
-        <v>-121</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.231</v>
+        <v>-0.005</v>
       </c>
       <c r="B5" t="n">
-        <v>0.01</v>
+        <v>-0.152</v>
       </c>
       <c r="C5" t="n">
-        <v>0.795</v>
+        <v>0.241</v>
       </c>
       <c r="D5" t="n">
-        <v>67</v>
+        <v>-128</v>
       </c>
       <c r="E5" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>-40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.227</v>
+        <v>-0.151</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.309</v>
+        <v>0.021</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.508</v>
+        <v>-0.358</v>
       </c>
       <c r="D6" t="n">
-        <v>124</v>
+        <v>-68</v>
       </c>
       <c r="E6" t="n">
-        <v>-2</v>
+        <v>-17</v>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.519</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.447</v>
+        <v>0.29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.052</v>
+        <v>-0.346</v>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>-105</v>
       </c>
       <c r="E7" t="n">
-        <v>31</v>
+        <v>-73</v>
       </c>
       <c r="F7" t="n">
-        <v>33</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.273</v>
+        <v>0.214</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.369</v>
+        <v>0.466</v>
       </c>
       <c r="C8" t="n">
-        <v>0.75</v>
+        <v>-0.063</v>
       </c>
       <c r="D8" t="n">
-        <v>175</v>
+        <v>-123</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>-52</v>
       </c>
       <c r="F8" t="n">
-        <v>170</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.001</v>
+        <v>0.218</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.118</v>
+        <v>-0.152</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.12</v>
+        <v>0.582</v>
       </c>
       <c r="D9" t="n">
-        <v>177</v>
+        <v>-143</v>
       </c>
       <c r="E9" t="n">
-        <v>-29</v>
+        <v>-79</v>
       </c>
       <c r="F9" t="n">
-        <v>-28</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.135</v>
+        <v>-0.524</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.238</v>
+        <v>-0.475</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.501</v>
+        <v>-0.028</v>
       </c>
       <c r="D10" t="n">
-        <v>-84</v>
+        <v>-26</v>
       </c>
       <c r="E10" t="n">
-        <v>-11</v>
+        <v>-44</v>
       </c>
       <c r="F10" t="n">
-        <v>157</v>
+        <v>-167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ddqn_train_eps & tested return current design
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.382</v>
+        <v>-0.299</v>
       </c>
       <c r="B1" t="n">
-        <v>0.537</v>
+        <v>0.175</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.121</v>
+        <v>-0.383</v>
       </c>
       <c r="D1" t="n">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E1" t="n">
-        <v>-34</v>
+        <v>69</v>
       </c>
       <c r="F1" t="n">
-        <v>36</v>
+        <v>-163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.508</v>
+        <v>-0.091</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.249</v>
+        <v>-0.063</v>
       </c>
       <c r="C2" t="n">
-        <v>0.233</v>
+        <v>-0.054</v>
       </c>
       <c r="D2" t="n">
-        <v>141</v>
+        <v>-89</v>
       </c>
       <c r="E2" t="n">
-        <v>-10</v>
+        <v>-63</v>
       </c>
       <c r="F2" t="n">
-        <v>127</v>
+        <v>-146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.095</v>
+        <v>-0.13</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.262</v>
+        <v>-0.056</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.276</v>
+        <v>-0.297</v>
       </c>
       <c r="D3" t="n">
-        <v>-148</v>
+        <v>-54</v>
       </c>
       <c r="E3" t="n">
-        <v>-79</v>
+        <v>44</v>
       </c>
       <c r="F3" t="n">
-        <v>-67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.596</v>
+        <v>-0.769</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.473</v>
+        <v>-0.29</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.035</v>
+        <v>-0.073</v>
       </c>
       <c r="D4" t="n">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="E4" t="n">
-        <v>-27</v>
+        <v>43</v>
       </c>
       <c r="F4" t="n">
-        <v>-36</v>
+        <v>-101</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.005</v>
+        <v>0.131</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.152</v>
+        <v>-0.145</v>
       </c>
       <c r="C5" t="n">
-        <v>0.241</v>
+        <v>0.282</v>
       </c>
       <c r="D5" t="n">
-        <v>-128</v>
+        <v>-62</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>-43</v>
       </c>
       <c r="F5" t="n">
-        <v>64</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.151</v>
+        <v>-0.167</v>
       </c>
       <c r="B6" t="n">
-        <v>0.021</v>
+        <v>-0.129</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.358</v>
+        <v>0.107</v>
       </c>
       <c r="D6" t="n">
-        <v>-68</v>
+        <v>85</v>
       </c>
       <c r="E6" t="n">
-        <v>-17</v>
+        <v>-52</v>
       </c>
       <c r="F6" t="n">
-        <v>-75</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.008999999999999999</v>
+        <v>-0.236</v>
       </c>
       <c r="B7" t="n">
-        <v>0.29</v>
+        <v>0.13</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.346</v>
+        <v>0.013</v>
       </c>
       <c r="D7" t="n">
-        <v>-105</v>
+        <v>111</v>
       </c>
       <c r="E7" t="n">
-        <v>-73</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.214</v>
+        <v>0.218</v>
       </c>
       <c r="B8" t="n">
-        <v>0.466</v>
+        <v>-0.165</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.063</v>
+        <v>0.914</v>
       </c>
       <c r="D8" t="n">
-        <v>-123</v>
+        <v>-72</v>
       </c>
       <c r="E8" t="n">
-        <v>-52</v>
+        <v>36</v>
       </c>
       <c r="F8" t="n">
-        <v>55</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.218</v>
+        <v>-0.579</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.152</v>
+        <v>0.202</v>
       </c>
       <c r="C9" t="n">
-        <v>0.582</v>
+        <v>-0.078</v>
       </c>
       <c r="D9" t="n">
-        <v>-143</v>
+        <v>-110</v>
       </c>
       <c r="E9" t="n">
-        <v>-79</v>
+        <v>-7</v>
       </c>
       <c r="F9" t="n">
-        <v>-125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.524</v>
+        <v>0.091</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.475</v>
+        <v>-0.057</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.028</v>
+        <v>0.056</v>
       </c>
       <c r="D10" t="n">
-        <v>-26</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>-44</v>
+        <v>48</v>
       </c>
       <c r="F10" t="n">
-        <v>-167</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed axis length action space negative value
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.209</v>
+        <v>-0.376</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.371</v>
+        <v>0.155</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.344</v>
+        <v>0.444</v>
       </c>
       <c r="D1" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E1" t="n">
-        <v>-20</v>
+        <v>48</v>
       </c>
       <c r="F1" t="n">
-        <v>47</v>
+        <v>-175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.128</v>
+        <v>-0.165</v>
       </c>
       <c r="B2" t="n">
-        <v>0.189</v>
+        <v>0.181</v>
       </c>
       <c r="C2" t="n">
-        <v>0.349</v>
+        <v>0.662</v>
       </c>
       <c r="D2" t="n">
-        <v>-146</v>
+        <v>-61</v>
       </c>
       <c r="E2" t="n">
-        <v>75</v>
+        <v>-13</v>
       </c>
       <c r="F2" t="n">
-        <v>-129</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.488</v>
+        <v>0.591</v>
       </c>
       <c r="B3" t="n">
-        <v>0.206</v>
+        <v>-0.236</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.006</v>
+        <v>0.193</v>
       </c>
       <c r="D3" t="n">
-        <v>-3</v>
+        <v>-61</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>-25</v>
       </c>
       <c r="F3" t="n">
-        <v>-148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.463</v>
+        <v>0.188</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.095</v>
+        <v>-0.002</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.047</v>
+        <v>0.628</v>
       </c>
       <c r="D4" t="n">
-        <v>-72</v>
+        <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>47</v>
+        <v>-59</v>
       </c>
       <c r="F4" t="n">
-        <v>-158</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.095</v>
+        <v>-0.463</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.078</v>
+        <v>0.248</v>
       </c>
       <c r="C5" t="n">
-        <v>0.475</v>
+        <v>0.371</v>
       </c>
       <c r="D5" t="n">
-        <v>-147</v>
+        <v>-39</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>-10</v>
       </c>
       <c r="F5" t="n">
-        <v>107</v>
+        <v>-107</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.331</v>
+        <v>-0.14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.258</v>
+        <v>0.057</v>
       </c>
       <c r="C6" t="n">
-        <v>0.154</v>
+        <v>0.432</v>
       </c>
       <c r="D6" t="n">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="E6" t="n">
-        <v>60</v>
+        <v>-1</v>
       </c>
       <c r="F6" t="n">
-        <v>-75</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.5590000000000001</v>
+        <v>-0.168</v>
       </c>
       <c r="B7" t="n">
-        <v>0.007</v>
+        <v>-0.447</v>
       </c>
       <c r="C7" t="n">
-        <v>0.175</v>
+        <v>0.469</v>
       </c>
       <c r="D7" t="n">
-        <v>-67</v>
+        <v>51</v>
       </c>
       <c r="E7" t="n">
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-38</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.375</v>
+        <v>-0.333</v>
       </c>
       <c r="B8" t="n">
-        <v>0.142</v>
+        <v>-0.052</v>
       </c>
       <c r="C8" t="n">
-        <v>0.11</v>
+        <v>-0.151</v>
       </c>
       <c r="D8" t="n">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="E8" t="n">
         <v>-1</v>
       </c>
       <c r="F8" t="n">
-        <v>86</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.09</v>
+        <v>-0.059</v>
       </c>
       <c r="B9" t="n">
-        <v>0.312</v>
+        <v>-0.026</v>
       </c>
       <c r="C9" t="n">
-        <v>0.522</v>
+        <v>0.602</v>
       </c>
       <c r="D9" t="n">
-        <v>99</v>
+        <v>-118</v>
       </c>
       <c r="E9" t="n">
-        <v>-34</v>
+        <v>58</v>
       </c>
       <c r="F9" t="n">
-        <v>-141</v>
+        <v>-157</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.195</v>
+        <v>-0.369</v>
       </c>
       <c r="B10" t="n">
-        <v>0.179</v>
+        <v>-0.078</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.028</v>
+        <v>0.312</v>
       </c>
       <c r="D10" t="n">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="E10" t="n">
-        <v>-41</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>-56</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 3dof can train
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.376</v>
+        <v>0.428</v>
       </c>
       <c r="B1" t="n">
-        <v>0.155</v>
+        <v>-0.112</v>
       </c>
       <c r="C1" t="n">
-        <v>0.444</v>
+        <v>-0.2</v>
       </c>
       <c r="D1" t="n">
-        <v>92</v>
+        <v>-1</v>
       </c>
       <c r="E1" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F1" t="n">
-        <v>-175</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.165</v>
+        <v>0.418</v>
       </c>
       <c r="B2" t="n">
-        <v>0.181</v>
+        <v>0.259</v>
       </c>
       <c r="C2" t="n">
-        <v>0.662</v>
+        <v>0.148</v>
       </c>
       <c r="D2" t="n">
-        <v>-61</v>
+        <v>165</v>
       </c>
       <c r="E2" t="n">
         <v>-13</v>
       </c>
       <c r="F2" t="n">
-        <v>21</v>
+        <v>-154</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.591</v>
+        <v>-0.219</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.236</v>
+        <v>-0.516</v>
       </c>
       <c r="C3" t="n">
-        <v>0.193</v>
+        <v>0.31</v>
       </c>
       <c r="D3" t="n">
-        <v>-61</v>
+        <v>-38</v>
       </c>
       <c r="E3" t="n">
-        <v>-25</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>156</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.188</v>
+        <v>0.162</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.002</v>
+        <v>0.384</v>
       </c>
       <c r="C4" t="n">
-        <v>0.628</v>
+        <v>0.107</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="E4" t="n">
-        <v>-59</v>
+        <v>28</v>
       </c>
       <c r="F4" t="n">
-        <v>158</v>
+        <v>-79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.463</v>
+        <v>-0.296</v>
       </c>
       <c r="B5" t="n">
-        <v>0.248</v>
+        <v>0.232</v>
       </c>
       <c r="C5" t="n">
-        <v>0.371</v>
+        <v>-0.135</v>
       </c>
       <c r="D5" t="n">
-        <v>-39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="n">
-        <v>-10</v>
+        <v>34</v>
       </c>
       <c r="F5" t="n">
-        <v>-107</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.14</v>
+        <v>0.272</v>
       </c>
       <c r="B6" t="n">
-        <v>0.057</v>
+        <v>0.235</v>
       </c>
       <c r="C6" t="n">
-        <v>0.432</v>
+        <v>-0.074</v>
       </c>
       <c r="D6" t="n">
-        <v>156</v>
+        <v>-82</v>
       </c>
       <c r="E6" t="n">
-        <v>-1</v>
+        <v>33</v>
       </c>
       <c r="F6" t="n">
-        <v>-10</v>
+        <v>-154</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.168</v>
+        <v>-0.191</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.447</v>
+        <v>-0.194</v>
       </c>
       <c r="C7" t="n">
-        <v>0.469</v>
+        <v>0.725</v>
       </c>
       <c r="D7" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F7" t="n">
-        <v>-134</v>
+        <v>-121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.333</v>
+        <v>0.179</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.052</v>
+        <v>0.283</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.151</v>
+        <v>-0.161</v>
       </c>
       <c r="D8" t="n">
-        <v>98</v>
+        <v>-131</v>
       </c>
       <c r="E8" t="n">
-        <v>-1</v>
+        <v>-51</v>
       </c>
       <c r="F8" t="n">
-        <v>-19</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.059</v>
+        <v>-0.242</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.026</v>
+        <v>0.269</v>
       </c>
       <c r="C9" t="n">
-        <v>0.602</v>
+        <v>0.167</v>
       </c>
       <c r="D9" t="n">
-        <v>-118</v>
+        <v>100</v>
       </c>
       <c r="E9" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F9" t="n">
-        <v>-157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.369</v>
+        <v>-0.154</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.078</v>
+        <v>-0.173</v>
       </c>
       <c r="C10" t="n">
-        <v>0.312</v>
+        <v>0.489</v>
       </c>
       <c r="D10" t="n">
-        <v>31</v>
+        <v>-89</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>-5</v>
       </c>
       <c r="F10" t="n">
-        <v>173</v>
+        <v>-177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use virtual links, 5 dof no problem, but 4dof
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.428</v>
+        <v>-0.184</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.112</v>
+        <v>-0.05</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.2</v>
+        <v>0.729</v>
       </c>
       <c r="D1" t="n">
-        <v>-1</v>
+        <v>170</v>
       </c>
       <c r="E1" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F1" t="n">
-        <v>-40</v>
+        <v>-108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.418</v>
+        <v>-0.008</v>
       </c>
       <c r="B2" t="n">
-        <v>0.259</v>
+        <v>0.212</v>
       </c>
       <c r="C2" t="n">
-        <v>0.148</v>
+        <v>-0.133</v>
       </c>
       <c r="D2" t="n">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="E2" t="n">
-        <v>-13</v>
+        <v>71</v>
       </c>
       <c r="F2" t="n">
-        <v>-154</v>
+        <v>-104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.219</v>
+        <v>0.074</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.516</v>
+        <v>-0.281</v>
       </c>
       <c r="C3" t="n">
-        <v>0.31</v>
+        <v>0.004</v>
       </c>
       <c r="D3" t="n">
-        <v>-38</v>
+        <v>142</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>-46</v>
       </c>
       <c r="F3" t="n">
-        <v>-9</v>
+        <v>-132</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.162</v>
+        <v>0.294</v>
       </c>
       <c r="B4" t="n">
-        <v>0.384</v>
+        <v>0.075</v>
       </c>
       <c r="C4" t="n">
-        <v>0.107</v>
+        <v>-0.101</v>
       </c>
       <c r="D4" t="n">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F4" t="n">
-        <v>-79</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.296</v>
+        <v>-0.735</v>
       </c>
       <c r="B5" t="n">
-        <v>0.232</v>
+        <v>-0.157</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.135</v>
+        <v>0.428</v>
       </c>
       <c r="D5" t="n">
-        <v>38</v>
+        <v>-4</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>-23</v>
       </c>
       <c r="F5" t="n">
-        <v>-70</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.272</v>
+        <v>-0.314</v>
       </c>
       <c r="B6" t="n">
-        <v>0.235</v>
+        <v>0.024</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.074</v>
+        <v>-0.339</v>
       </c>
       <c r="D6" t="n">
-        <v>-82</v>
+        <v>-113</v>
       </c>
       <c r="E6" t="n">
-        <v>33</v>
+        <v>-7</v>
       </c>
       <c r="F6" t="n">
-        <v>-154</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.191</v>
+        <v>-0.122</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.194</v>
+        <v>-0.473</v>
       </c>
       <c r="C7" t="n">
-        <v>0.725</v>
+        <v>0.514</v>
       </c>
       <c r="D7" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E7" t="n">
-        <v>77</v>
+        <v>-77</v>
       </c>
       <c r="F7" t="n">
-        <v>-121</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.179</v>
+        <v>0.173</v>
       </c>
       <c r="B8" t="n">
-        <v>0.283</v>
+        <v>-0.123</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.161</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>-131</v>
+        <v>137</v>
       </c>
       <c r="E8" t="n">
-        <v>-51</v>
+        <v>84</v>
       </c>
       <c r="F8" t="n">
-        <v>-36</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.242</v>
+        <v>0.111</v>
       </c>
       <c r="B9" t="n">
-        <v>0.269</v>
+        <v>-0.317</v>
       </c>
       <c r="C9" t="n">
-        <v>0.167</v>
+        <v>0.057</v>
       </c>
       <c r="D9" t="n">
-        <v>100</v>
+        <v>-3</v>
       </c>
       <c r="E9" t="n">
-        <v>49</v>
+        <v>-87</v>
       </c>
       <c r="F9" t="n">
-        <v>132</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.154</v>
+        <v>0.189</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.173</v>
+        <v>0.595</v>
       </c>
       <c r="C10" t="n">
-        <v>0.489</v>
+        <v>0.174</v>
       </c>
       <c r="D10" t="n">
-        <v>-89</v>
+        <v>-86</v>
       </c>
       <c r="E10" t="n">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>-177</v>
+        <v>-81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed observation & reward
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.184</v>
+        <v>0.115</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.05</v>
+        <v>-0.109</v>
       </c>
       <c r="C1" t="n">
-        <v>0.729</v>
+        <v>-0.321</v>
       </c>
       <c r="D1" t="n">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="E1" t="n">
-        <v>17</v>
+        <v>-19</v>
       </c>
       <c r="F1" t="n">
-        <v>-108</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.008</v>
+        <v>0.203</v>
       </c>
       <c r="B2" t="n">
-        <v>0.212</v>
+        <v>0.501</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.133</v>
+        <v>-0.024</v>
       </c>
       <c r="D2" t="n">
-        <v>111</v>
+        <v>-139</v>
       </c>
       <c r="E2" t="n">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>-104</v>
+        <v>-169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.074</v>
+        <v>0.038</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.281</v>
+        <v>0.061</v>
       </c>
       <c r="C3" t="n">
-        <v>0.004</v>
+        <v>0.866</v>
       </c>
       <c r="D3" t="n">
-        <v>142</v>
+        <v>-100</v>
       </c>
       <c r="E3" t="n">
-        <v>-46</v>
+        <v>55</v>
       </c>
       <c r="F3" t="n">
-        <v>-132</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.294</v>
+        <v>-0.239</v>
       </c>
       <c r="B4" t="n">
-        <v>0.075</v>
+        <v>-0.028</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.101</v>
+        <v>0.706</v>
       </c>
       <c r="D4" t="n">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="E4" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>101</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.735</v>
+        <v>0.126</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.157</v>
+        <v>-0.125</v>
       </c>
       <c r="C5" t="n">
-        <v>0.428</v>
+        <v>0.294</v>
       </c>
       <c r="D5" t="n">
-        <v>-4</v>
+        <v>96</v>
       </c>
       <c r="E5" t="n">
-        <v>-23</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.314</v>
+        <v>0.12</v>
       </c>
       <c r="B6" t="n">
-        <v>0.024</v>
+        <v>0.048</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.339</v>
+        <v>0.305</v>
       </c>
       <c r="D6" t="n">
-        <v>-113</v>
+        <v>36</v>
       </c>
       <c r="E6" t="n">
-        <v>-7</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.122</v>
+        <v>-0.075</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.473</v>
+        <v>0.01</v>
       </c>
       <c r="C7" t="n">
-        <v>0.514</v>
+        <v>0.82</v>
       </c>
       <c r="D7" t="n">
-        <v>71</v>
+        <v>-83</v>
       </c>
       <c r="E7" t="n">
-        <v>-77</v>
+        <v>-51</v>
       </c>
       <c r="F7" t="n">
-        <v>-81</v>
+        <v>-157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.173</v>
+        <v>-0.074</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.123</v>
+        <v>-0.207</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.189</v>
       </c>
       <c r="D8" t="n">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="E8" t="n">
-        <v>84</v>
+        <v>-50</v>
       </c>
       <c r="F8" t="n">
-        <v>-103</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.111</v>
+        <v>0.299</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.317</v>
+        <v>-0.232</v>
       </c>
       <c r="C9" t="n">
-        <v>0.057</v>
+        <v>-0.12</v>
       </c>
       <c r="D9" t="n">
-        <v>-3</v>
+        <v>88</v>
       </c>
       <c r="E9" t="n">
-        <v>-87</v>
+        <v>-66</v>
       </c>
       <c r="F9" t="n">
-        <v>56</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.189</v>
+        <v>-0.223</v>
       </c>
       <c r="B10" t="n">
-        <v>0.595</v>
+        <v>-0.082</v>
       </c>
       <c r="C10" t="n">
-        <v>0.174</v>
+        <v>0.187</v>
       </c>
       <c r="D10" t="n">
-        <v>-86</v>
+        <v>139</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>-24</v>
       </c>
       <c r="F10" t="n">
-        <v>-81</v>
+        <v>-51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
learning rate & inf reward fixed
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.078</v>
+        <v>0.315</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.074</v>
+        <v>0.279</v>
       </c>
       <c r="C1" t="n">
-        <v>0.21</v>
+        <v>-0.479</v>
       </c>
       <c r="D1" t="n">
-        <v>-148</v>
+        <v>-61</v>
       </c>
       <c r="E1" t="n">
-        <v>33</v>
+        <v>-65</v>
       </c>
       <c r="F1" t="n">
-        <v>169</v>
+        <v>-112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.337</v>
+        <v>0.011</v>
       </c>
       <c r="B2" t="n">
-        <v>0.022</v>
+        <v>0.141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>157</v>
+        <v>-70</v>
       </c>
       <c r="E2" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
-        <v>156</v>
+        <v>-71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.132</v>
+        <v>0.098</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.17</v>
+        <v>-0.171</v>
       </c>
       <c r="C3" t="n">
-        <v>0.516</v>
+        <v>0.381</v>
       </c>
       <c r="D3" t="n">
-        <v>-114</v>
+        <v>-67</v>
       </c>
       <c r="E3" t="n">
-        <v>-55</v>
+        <v>-16</v>
       </c>
       <c r="F3" t="n">
-        <v>-153</v>
+        <v>-139</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.121</v>
+        <v>0.521</v>
       </c>
       <c r="B4" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.294</v>
       </c>
       <c r="C4" t="n">
-        <v>0.175</v>
+        <v>-0.073</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E4" t="n">
-        <v>-58</v>
+        <v>-43</v>
       </c>
       <c r="F4" t="n">
-        <v>91</v>
+        <v>-156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.335</v>
+        <v>0.073</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.295</v>
+        <v>-0.171</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4</v>
+        <v>0.869</v>
       </c>
       <c r="D5" t="n">
-        <v>55</v>
+        <v>-122</v>
       </c>
       <c r="E5" t="n">
-        <v>-42</v>
+        <v>-15</v>
       </c>
       <c r="F5" t="n">
-        <v>-148</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.144</v>
+        <v>0.62</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.283</v>
+        <v>0.08</v>
       </c>
       <c r="C6" t="n">
-        <v>0.27</v>
+        <v>0.57</v>
       </c>
       <c r="D6" t="n">
-        <v>-179</v>
+        <v>-57</v>
       </c>
       <c r="E6" t="n">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F6" t="n">
-        <v>-15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.173</v>
+        <v>0.067</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.119</v>
+        <v>0.223</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.08</v>
+        <v>0.019</v>
       </c>
       <c r="D7" t="n">
-        <v>-91</v>
+        <v>129</v>
       </c>
       <c r="E7" t="n">
-        <v>-1</v>
+        <v>-21</v>
       </c>
       <c r="F7" t="n">
-        <v>-146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.133</v>
+        <v>0.167</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.052</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.198</v>
+        <v>0.587</v>
       </c>
       <c r="D8" t="n">
-        <v>-143</v>
+        <v>-155</v>
       </c>
       <c r="E8" t="n">
-        <v>-3</v>
+        <v>50</v>
       </c>
       <c r="F8" t="n">
-        <v>-134</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.07199999999999999</v>
+        <v>0.62</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.269</v>
+        <v>0.08</v>
       </c>
       <c r="C9" t="n">
-        <v>0.654</v>
+        <v>0.57</v>
       </c>
       <c r="D9" t="n">
-        <v>124</v>
+        <v>-57</v>
       </c>
       <c r="E9" t="n">
-        <v>-35</v>
+        <v>25</v>
       </c>
       <c r="F9" t="n">
-        <v>-12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.027</v>
+        <v>-0.197</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.474</v>
+        <v>0.113</v>
       </c>
       <c r="C10" t="n">
-        <v>0.266</v>
+        <v>-0.351</v>
       </c>
       <c r="D10" t="n">
-        <v>96</v>
+        <v>-97</v>
       </c>
       <c r="E10" t="n">
-        <v>27</v>
+        <v>-44</v>
       </c>
       <c r="F10" t="n">
-        <v>96</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed tested error & reward
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.045</v>
+        <v>-0.008</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.267</v>
+        <v>-0.448</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.336</v>
+        <v>-0.212</v>
       </c>
       <c r="D1" t="n">
-        <v>-89</v>
+        <v>97</v>
       </c>
       <c r="E1" t="n">
-        <v>-72</v>
+        <v>59</v>
       </c>
       <c r="F1" t="n">
-        <v>-109</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.178</v>
+        <v>0.153</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.213</v>
+        <v>-0.041</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.37</v>
+        <v>0.388</v>
       </c>
       <c r="D2" t="n">
-        <v>174</v>
+        <v>-89</v>
       </c>
       <c r="E2" t="n">
-        <v>-40</v>
+        <v>55</v>
       </c>
       <c r="F2" t="n">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.313</v>
+        <v>-0.297</v>
       </c>
       <c r="B3" t="n">
-        <v>0.121</v>
+        <v>-0.169</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.05</v>
+        <v>0.243</v>
       </c>
       <c r="D3" t="n">
-        <v>41</v>
+        <v>-108</v>
       </c>
       <c r="E3" t="n">
-        <v>-32</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>-38</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.015</v>
+        <v>-0.173</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.193</v>
+        <v>-0.08</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.318</v>
+        <v>0.599</v>
       </c>
       <c r="D4" t="n">
-        <v>34</v>
+        <v>-33</v>
       </c>
       <c r="E4" t="n">
-        <v>-42</v>
+        <v>21</v>
       </c>
       <c r="F4" t="n">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.119</v>
+        <v>0.2</v>
       </c>
       <c r="B5" t="n">
-        <v>0.416</v>
+        <v>-0.259</v>
       </c>
       <c r="C5" t="n">
-        <v>0.398</v>
+        <v>0.555</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E5" t="n">
-        <v>68</v>
+        <v>-44</v>
       </c>
       <c r="F5" t="n">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.241</v>
+        <v>0.156</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.335</v>
+        <v>-0.002</v>
       </c>
       <c r="C6" t="n">
-        <v>0.285</v>
+        <v>0.598</v>
       </c>
       <c r="D6" t="n">
-        <v>-142</v>
+        <v>58</v>
       </c>
       <c r="E6" t="n">
-        <v>-54</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>-153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.01</v>
+        <v>-0.134</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.276</v>
+        <v>-0.322</v>
       </c>
       <c r="C7" t="n">
-        <v>0.63</v>
+        <v>0.576</v>
       </c>
       <c r="D7" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E7" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" t="n">
-        <v>-100</v>
+        <v>-107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.112</v>
+        <v>-0.061</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.25</v>
+        <v>-0.162</v>
       </c>
       <c r="C8" t="n">
-        <v>0.423</v>
+        <v>0.519</v>
       </c>
       <c r="D8" t="n">
-        <v>-98</v>
+        <v>89</v>
       </c>
       <c r="E8" t="n">
-        <v>29</v>
+        <v>-16</v>
       </c>
       <c r="F8" t="n">
-        <v>125</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.042</v>
+        <v>0.205</v>
       </c>
       <c r="B9" t="n">
-        <v>0.183</v>
+        <v>-0.351</v>
       </c>
       <c r="C9" t="n">
-        <v>0.352</v>
+        <v>0.267</v>
       </c>
       <c r="D9" t="n">
-        <v>-150</v>
+        <v>97</v>
       </c>
       <c r="E9" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.185</v>
+        <v>-0.372</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.055</v>
+        <v>0.004</v>
       </c>
       <c r="C10" t="n">
-        <v>0.109</v>
+        <v>0.235</v>
       </c>
       <c r="D10" t="n">
-        <v>62</v>
+        <v>-40</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F10" t="n">
-        <v>81</v>
+        <v>-121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed tb.add_scalar  input data type
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,99 +423,99 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.145</v>
+        <v>0.143</v>
       </c>
       <c r="B1" t="n">
-        <v>0.284</v>
+        <v>-0.221</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.11</v>
+        <v>0.067</v>
       </c>
       <c r="D1" t="n">
-        <v>-44</v>
+        <v>-55</v>
       </c>
       <c r="E1" t="n">
-        <v>7</v>
+        <v>-36</v>
       </c>
       <c r="F1" t="n">
-        <v>29</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.022</v>
+        <v>-0.339</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.313</v>
+        <v>-0.334</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.277</v>
+        <v>0.3</v>
       </c>
       <c r="D2" t="n">
-        <v>-18</v>
+        <v>-113</v>
       </c>
       <c r="E2" t="n">
-        <v>-72</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.394</v>
+        <v>-0.188</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.098</v>
+        <v>0.045</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.057</v>
+        <v>0.542</v>
       </c>
       <c r="D3" t="n">
-        <v>-85</v>
+        <v>82</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="F3" t="n">
-        <v>170</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.049</v>
+        <v>-0.051</v>
       </c>
       <c r="B4" t="n">
-        <v>0.28</v>
+        <v>0.172</v>
       </c>
       <c r="C4" t="n">
-        <v>0.705</v>
+        <v>-0.039</v>
       </c>
       <c r="D4" t="n">
-        <v>-99</v>
+        <v>-72</v>
       </c>
       <c r="E4" t="n">
-        <v>-42</v>
+        <v>-31</v>
       </c>
       <c r="F4" t="n">
-        <v>-57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.097</v>
+        <v>-0.36</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.31</v>
+        <v>0.016</v>
       </c>
       <c r="C5" t="n">
-        <v>0.579</v>
+        <v>0.472</v>
       </c>
       <c r="D5" t="n">
-        <v>-64</v>
+        <v>29</v>
       </c>
       <c r="E5" t="n">
-        <v>60</v>
+        <v>-9</v>
       </c>
       <c r="F5" t="n">
         <v>-74</v>
@@ -523,102 +523,102 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.29</v>
+        <v>0.201</v>
       </c>
       <c r="B6" t="n">
-        <v>0.066</v>
+        <v>-0.292</v>
       </c>
       <c r="C6" t="n">
-        <v>0.42</v>
+        <v>-0.011</v>
       </c>
       <c r="D6" t="n">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n">
-        <v>-47</v>
+        <v>80</v>
       </c>
       <c r="F6" t="n">
-        <v>129</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.246</v>
+        <v>0.124</v>
       </c>
       <c r="B7" t="n">
-        <v>0.027</v>
+        <v>-0.079</v>
       </c>
       <c r="C7" t="n">
-        <v>0.713</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="E7" t="n">
-        <v>-64</v>
+        <v>22</v>
       </c>
       <c r="F7" t="n">
-        <v>45</v>
+        <v>-176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.07099999999999999</v>
+        <v>0.064</v>
       </c>
       <c r="B8" t="n">
-        <v>0.079</v>
+        <v>0.062</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.437</v>
+        <v>0.408</v>
       </c>
       <c r="D8" t="n">
-        <v>-51</v>
+        <v>88</v>
       </c>
       <c r="E8" t="n">
-        <v>-11</v>
+        <v>23</v>
       </c>
       <c r="F8" t="n">
-        <v>-101</v>
+        <v>-112</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.343</v>
+        <v>-0.139</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.588</v>
+        <v>-0.37</v>
       </c>
       <c r="C9" t="n">
-        <v>0.017</v>
+        <v>0.165</v>
       </c>
       <c r="D9" t="n">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E9" t="n">
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
-        <v>-94</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.107</v>
+        <v>-0.409</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.08</v>
+        <v>0.038</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.222</v>
+        <v>-0.044</v>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>-157</v>
       </c>
       <c r="E10" t="n">
-        <v>-21</v>
+        <v>-10</v>
       </c>
       <c r="F10" t="n">
-        <v>-81</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add train tensorboard record & test model
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.41</v>
+        <v>-0.163</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.144</v>
+        <v>-0.108</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.228</v>
+        <v>0.212</v>
       </c>
       <c r="D1" t="n">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="E1" t="n">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="F1" t="n">
-        <v>-154</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.222</v>
+        <v>0.397</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.095</v>
+        <v>-0.198</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.142</v>
+        <v>-0.455</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>-7</v>
       </c>
       <c r="E2" t="n">
-        <v>-7</v>
+        <v>-30</v>
       </c>
       <c r="F2" t="n">
-        <v>61</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.188</v>
+        <v>-0.308</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.187</v>
+        <v>-0.233</v>
       </c>
       <c r="C3" t="n">
-        <v>0.064</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F3" t="n">
-        <v>118</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.094</v>
+        <v>-0.036</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.08400000000000001</v>
+        <v>-0.9379999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>0.615</v>
+        <v>0.119</v>
       </c>
       <c r="D4" t="n">
-        <v>-149</v>
+        <v>-20</v>
       </c>
       <c r="E4" t="n">
-        <v>-8</v>
+        <v>40</v>
       </c>
       <c r="F4" t="n">
-        <v>-162</v>
+        <v>-54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.073</v>
+        <v>-0.22</v>
       </c>
       <c r="B5" t="n">
-        <v>0.285</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>0.351</v>
+        <v>0.192</v>
       </c>
       <c r="D5" t="n">
-        <v>-160</v>
+        <v>-146</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F5" t="n">
-        <v>-44</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.112</v>
+        <v>0.128</v>
       </c>
       <c r="B6" t="n">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.306</v>
+        <v>0.145</v>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>-21</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>-10</v>
       </c>
       <c r="F6" t="n">
-        <v>-123</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.137</v>
+        <v>0.092</v>
       </c>
       <c r="B7" t="n">
-        <v>0.331</v>
+        <v>-0.152</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.049</v>
+        <v>-0.303</v>
       </c>
       <c r="D7" t="n">
-        <v>69</v>
+        <v>-25</v>
       </c>
       <c r="E7" t="n">
-        <v>-23</v>
+        <v>-26</v>
       </c>
       <c r="F7" t="n">
-        <v>-90</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.152</v>
+        <v>-0.261</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.122</v>
+        <v>-0.316</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7</v>
+        <v>0.701</v>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-49</v>
       </c>
       <c r="F8" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.619</v>
+        <v>-0.341</v>
       </c>
       <c r="B9" t="n">
-        <v>0.046</v>
+        <v>-0.215</v>
       </c>
       <c r="C9" t="n">
-        <v>0.048</v>
+        <v>0.717</v>
       </c>
       <c r="D9" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E9" t="n">
-        <v>23</v>
+        <v>-60</v>
       </c>
       <c r="F9" t="n">
-        <v>168</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.383</v>
+        <v>-0.136</v>
       </c>
       <c r="B10" t="n">
-        <v>0.518</v>
+        <v>0.235</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002</v>
+        <v>0.1</v>
       </c>
       <c r="D10" t="n">
-        <v>-169</v>
+        <v>-137</v>
       </c>
       <c r="E10" t="n">
-        <v>-9</v>
+        <v>-14</v>
       </c>
       <c r="F10" t="n">
-        <v>116</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DRL general select function
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.163</v>
+        <v>-0.017</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.108</v>
+        <v>0.553</v>
       </c>
       <c r="C1" t="n">
-        <v>0.212</v>
+        <v>0.605</v>
       </c>
       <c r="D1" t="n">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="E1" t="n">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F1" t="n">
-        <v>-78</v>
+        <v>-91</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.397</v>
+        <v>-0.336</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.198</v>
+        <v>0.215</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.455</v>
+        <v>0.606</v>
       </c>
       <c r="D2" t="n">
-        <v>-7</v>
+        <v>122</v>
       </c>
       <c r="E2" t="n">
-        <v>-30</v>
+        <v>-57</v>
       </c>
       <c r="F2" t="n">
-        <v>-6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.308</v>
+        <v>-0.449</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.233</v>
+        <v>-0.105</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6840000000000001</v>
+        <v>-0.089</v>
       </c>
       <c r="D3" t="n">
-        <v>94</v>
+        <v>-132</v>
       </c>
       <c r="E3" t="n">
-        <v>85</v>
+        <v>-6</v>
       </c>
       <c r="F3" t="n">
-        <v>42</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.036</v>
+        <v>-0.019</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.9379999999999999</v>
+        <v>-0.188</v>
       </c>
       <c r="C4" t="n">
-        <v>0.119</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>-20</v>
+        <v>52</v>
       </c>
       <c r="E4" t="n">
-        <v>40</v>
+        <v>-68</v>
       </c>
       <c r="F4" t="n">
-        <v>-54</v>
+        <v>-89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.22</v>
+        <v>-0.176</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.07199999999999999</v>
+        <v>-0.007</v>
       </c>
       <c r="C5" t="n">
-        <v>0.192</v>
+        <v>0.695</v>
       </c>
       <c r="D5" t="n">
-        <v>-146</v>
+        <v>171</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F5" t="n">
-        <v>-133</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.128</v>
+        <v>0.176</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7</v>
+        <v>0.051</v>
       </c>
       <c r="C6" t="n">
-        <v>0.145</v>
+        <v>0.797</v>
       </c>
       <c r="D6" t="n">
-        <v>-21</v>
+        <v>-1</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>176</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.092</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.152</v>
+        <v>-0.296</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.303</v>
+        <v>0.446</v>
       </c>
       <c r="D7" t="n">
-        <v>-25</v>
+        <v>141</v>
       </c>
       <c r="E7" t="n">
-        <v>-26</v>
+        <v>17</v>
       </c>
       <c r="F7" t="n">
-        <v>38</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.261</v>
+        <v>0.429</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.316</v>
+        <v>0.131</v>
       </c>
       <c r="C8" t="n">
-        <v>0.701</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>122</v>
+        <v>-30</v>
       </c>
       <c r="E8" t="n">
-        <v>-49</v>
+        <v>57</v>
       </c>
       <c r="F8" t="n">
-        <v>97</v>
+        <v>-149</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.341</v>
+        <v>0.046</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.215</v>
+        <v>0.064</v>
       </c>
       <c r="C9" t="n">
-        <v>0.717</v>
+        <v>0.315</v>
       </c>
       <c r="D9" t="n">
-        <v>93</v>
+        <v>-55</v>
       </c>
       <c r="E9" t="n">
-        <v>-60</v>
+        <v>42</v>
       </c>
       <c r="F9" t="n">
-        <v>14</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.136</v>
+        <v>0.332</v>
       </c>
       <c r="B10" t="n">
-        <v>0.235</v>
+        <v>-0.152</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1</v>
+        <v>-0.068</v>
       </c>
       <c r="D10" t="n">
-        <v>-137</v>
+        <v>93</v>
       </c>
       <c r="E10" t="n">
-        <v>-14</v>
+        <v>-5</v>
       </c>
       <c r="F10" t="n">
-        <v>19</v>
+        <v>-143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
修改save model & read 的路徑
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.017</v>
+        <v>0.244</v>
       </c>
       <c r="B1" t="n">
-        <v>0.553</v>
+        <v>0.093</v>
       </c>
       <c r="C1" t="n">
-        <v>0.605</v>
+        <v>0.046</v>
       </c>
       <c r="D1" t="n">
-        <v>53</v>
+        <v>-48</v>
       </c>
       <c r="E1" t="n">
-        <v>45</v>
+        <v>-1</v>
       </c>
       <c r="F1" t="n">
-        <v>-91</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.336</v>
+        <v>0.227</v>
       </c>
       <c r="B2" t="n">
-        <v>0.215</v>
+        <v>-0.172</v>
       </c>
       <c r="C2" t="n">
-        <v>0.606</v>
+        <v>-0.357</v>
       </c>
       <c r="D2" t="n">
-        <v>122</v>
+        <v>-87</v>
       </c>
       <c r="E2" t="n">
-        <v>-57</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>-42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.449</v>
+        <v>0.207</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.105</v>
+        <v>0.437</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.089</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>-132</v>
+        <v>-173</v>
       </c>
       <c r="E3" t="n">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>-150</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.019</v>
+        <v>0.189</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.188</v>
+        <v>-0.325</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.047</v>
       </c>
       <c r="D4" t="n">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="E4" t="n">
-        <v>-68</v>
+        <v>35</v>
       </c>
       <c r="F4" t="n">
-        <v>-89</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.176</v>
+        <v>0.037</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.007</v>
+        <v>-0.187</v>
       </c>
       <c r="C5" t="n">
-        <v>0.695</v>
+        <v>0.385</v>
       </c>
       <c r="D5" t="n">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>-28</v>
       </c>
       <c r="F5" t="n">
-        <v>-48</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.176</v>
+        <v>-0.064</v>
       </c>
       <c r="B6" t="n">
-        <v>0.051</v>
+        <v>-0.11</v>
       </c>
       <c r="C6" t="n">
-        <v>0.797</v>
+        <v>0.492</v>
       </c>
       <c r="D6" t="n">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F6" t="n">
-        <v>-51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.08400000000000001</v>
+        <v>-0.134</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.296</v>
+        <v>0.043</v>
       </c>
       <c r="C7" t="n">
-        <v>0.446</v>
+        <v>0.359</v>
       </c>
       <c r="D7" t="n">
-        <v>141</v>
+        <v>-30</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.429</v>
+        <v>0.453</v>
       </c>
       <c r="B8" t="n">
-        <v>0.131</v>
+        <v>0.122</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.08400000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="D8" t="n">
-        <v>-30</v>
+        <v>44</v>
       </c>
       <c r="E8" t="n">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F8" t="n">
-        <v>-149</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.046</v>
+        <v>-0.276</v>
       </c>
       <c r="B9" t="n">
-        <v>0.064</v>
+        <v>0.079</v>
       </c>
       <c r="C9" t="n">
-        <v>0.315</v>
+        <v>0.101</v>
       </c>
       <c r="D9" t="n">
-        <v>-55</v>
+        <v>-7</v>
       </c>
       <c r="E9" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>84</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.332</v>
+        <v>0.2</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.152</v>
+        <v>0.035</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.068</v>
+        <v>-0.16</v>
       </c>
       <c r="D10" t="n">
-        <v>93</v>
+        <v>-13</v>
       </c>
       <c r="E10" t="n">
-        <v>-5</v>
+        <v>54</v>
       </c>
       <c r="F10" t="n">
-        <v>-143</v>
+        <v>-62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dqn& ddqn n_step_update
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.648</v>
+        <v>0.22</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.229</v>
+        <v>0.473</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.061</v>
+        <v>0.021</v>
       </c>
       <c r="D1" t="n">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="E1" t="n">
         <v>-14</v>
       </c>
       <c r="F1" t="n">
-        <v>-22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.334</v>
+        <v>-0.031</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.357</v>
+        <v>-0.162</v>
       </c>
       <c r="C2" t="n">
-        <v>0.078</v>
+        <v>0.604</v>
       </c>
       <c r="D2" t="n">
-        <v>-101</v>
+        <v>-178</v>
       </c>
       <c r="E2" t="n">
-        <v>-24</v>
+        <v>52</v>
       </c>
       <c r="F2" t="n">
-        <v>11</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.08699999999999999</v>
+        <v>0.361</v>
       </c>
       <c r="C3" t="n">
-        <v>0.251</v>
+        <v>0.32</v>
       </c>
       <c r="D3" t="n">
-        <v>-98</v>
+        <v>-38</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>-63</v>
       </c>
       <c r="F3" t="n">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.064</v>
+        <v>-0.03</v>
       </c>
       <c r="B4" t="n">
-        <v>0.211</v>
+        <v>-0.182</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.107</v>
       </c>
       <c r="D4" t="n">
-        <v>87</v>
+        <v>-156</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F4" t="n">
-        <v>-106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.192</v>
+        <v>0.114</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.232</v>
+        <v>0.183</v>
       </c>
       <c r="C5" t="n">
-        <v>0.509</v>
+        <v>0.459</v>
       </c>
       <c r="D5" t="n">
-        <v>66</v>
+        <v>-40</v>
       </c>
       <c r="E5" t="n">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>-42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.27</v>
+        <v>-0.169</v>
       </c>
       <c r="B6" t="n">
-        <v>0.043</v>
+        <v>-0.03</v>
       </c>
       <c r="C6" t="n">
-        <v>0.096</v>
+        <v>0.826</v>
       </c>
       <c r="D6" t="n">
-        <v>36</v>
+        <v>-89</v>
       </c>
       <c r="E6" t="n">
-        <v>-69</v>
+        <v>40</v>
       </c>
       <c r="F6" t="n">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.36</v>
+        <v>-0.121</v>
       </c>
       <c r="B7" t="n">
-        <v>0.054</v>
+        <v>0.121</v>
       </c>
       <c r="C7" t="n">
-        <v>0.331</v>
+        <v>0.436</v>
       </c>
       <c r="D7" t="n">
-        <v>-86</v>
+        <v>92</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>-138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.507</v>
+        <v>-0.035</v>
       </c>
       <c r="B8" t="n">
-        <v>0.222</v>
+        <v>0.173</v>
       </c>
       <c r="C8" t="n">
-        <v>0.259</v>
+        <v>-0.129</v>
       </c>
       <c r="D8" t="n">
-        <v>-91</v>
+        <v>-92</v>
       </c>
       <c r="E8" t="n">
-        <v>-24</v>
+        <v>50</v>
       </c>
       <c r="F8" t="n">
-        <v>73</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.413</v>
+        <v>0.018</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.054</v>
+        <v>-0.172</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.026</v>
+        <v>0.875</v>
       </c>
       <c r="D9" t="n">
-        <v>-70</v>
+        <v>74</v>
       </c>
       <c r="E9" t="n">
-        <v>-14</v>
+        <v>-62</v>
       </c>
       <c r="F9" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.423</v>
+        <v>-0.091</v>
       </c>
       <c r="B10" t="n">
-        <v>0.113</v>
+        <v>0.15</v>
       </c>
       <c r="C10" t="n">
-        <v>0.605</v>
+        <v>0.011</v>
       </c>
       <c r="D10" t="n">
-        <v>-111</v>
+        <v>53</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>-149</v>
+        <v>-163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed reward && set episode  cut off
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.22</v>
+        <v>0.348</v>
       </c>
       <c r="B1" t="n">
-        <v>0.473</v>
+        <v>-0.044</v>
       </c>
       <c r="C1" t="n">
-        <v>0.021</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="D1" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" t="n">
-        <v>-14</v>
+        <v>-8</v>
       </c>
       <c r="F1" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.031</v>
+        <v>0.06</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.162</v>
+        <v>0.224</v>
       </c>
       <c r="C2" t="n">
-        <v>0.604</v>
+        <v>0.505</v>
       </c>
       <c r="D2" t="n">
-        <v>-178</v>
+        <v>65</v>
       </c>
       <c r="E2" t="n">
-        <v>52</v>
+        <v>-54</v>
       </c>
       <c r="F2" t="n">
-        <v>142</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.325</v>
+        <v>0.09</v>
       </c>
       <c r="B3" t="n">
-        <v>0.361</v>
+        <v>-0.15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.32</v>
+        <v>0.513</v>
       </c>
       <c r="D3" t="n">
-        <v>-38</v>
+        <v>105</v>
       </c>
       <c r="E3" t="n">
-        <v>-63</v>
+        <v>74</v>
       </c>
       <c r="F3" t="n">
-        <v>126</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.03</v>
+        <v>0.016</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.182</v>
+        <v>0.381</v>
       </c>
       <c r="C4" t="n">
-        <v>0.107</v>
+        <v>-0.131</v>
       </c>
       <c r="D4" t="n">
-        <v>-156</v>
+        <v>145</v>
       </c>
       <c r="E4" t="n">
-        <v>58</v>
+        <v>-55</v>
       </c>
       <c r="F4" t="n">
-        <v>102</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.114</v>
+        <v>-0.116</v>
       </c>
       <c r="B5" t="n">
-        <v>0.183</v>
+        <v>-0.176</v>
       </c>
       <c r="C5" t="n">
-        <v>0.459</v>
+        <v>-0.21</v>
       </c>
       <c r="D5" t="n">
-        <v>-40</v>
+        <v>-126</v>
       </c>
       <c r="E5" t="n">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.169</v>
+        <v>-0.046</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.03</v>
+        <v>-0.136</v>
       </c>
       <c r="C6" t="n">
-        <v>0.826</v>
+        <v>0.443</v>
       </c>
       <c r="D6" t="n">
-        <v>-89</v>
+        <v>-46</v>
       </c>
       <c r="E6" t="n">
-        <v>40</v>
+        <v>-11</v>
       </c>
       <c r="F6" t="n">
-        <v>103</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.121</v>
+        <v>0.09</v>
       </c>
       <c r="B7" t="n">
-        <v>0.121</v>
+        <v>-0.493</v>
       </c>
       <c r="C7" t="n">
-        <v>0.436</v>
+        <v>0.331</v>
       </c>
       <c r="D7" t="n">
-        <v>92</v>
+        <v>-46</v>
       </c>
       <c r="E7" t="n">
-        <v>64</v>
+        <v>-70</v>
       </c>
       <c r="F7" t="n">
-        <v>-138</v>
+        <v>-113</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.035</v>
+        <v>-0.129</v>
       </c>
       <c r="B8" t="n">
-        <v>0.173</v>
+        <v>-0.012</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.129</v>
+        <v>0.098</v>
       </c>
       <c r="D8" t="n">
-        <v>-92</v>
+        <v>-178</v>
       </c>
       <c r="E8" t="n">
-        <v>50</v>
+        <v>-3</v>
       </c>
       <c r="F8" t="n">
-        <v>-4</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.018</v>
+        <v>-0.124</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.172</v>
+        <v>0.095</v>
       </c>
       <c r="C9" t="n">
-        <v>0.875</v>
+        <v>0.171</v>
       </c>
       <c r="D9" t="n">
-        <v>74</v>
+        <v>-173</v>
       </c>
       <c r="E9" t="n">
-        <v>-62</v>
+        <v>-4</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.091</v>
+        <v>-0.023</v>
       </c>
       <c r="B10" t="n">
-        <v>0.15</v>
+        <v>-0.027</v>
       </c>
       <c r="C10" t="n">
-        <v>0.011</v>
+        <v>0.363</v>
       </c>
       <c r="D10" t="n">
-        <v>53</v>
+        <v>-89</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="F10" t="n">
-        <v>-163</v>
+        <v>-36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed read urdf error
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.124</v>
+        <v>0.028</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.073</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="C1" t="n">
-        <v>0.603</v>
+        <v>0.844</v>
       </c>
       <c r="D1" t="n">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="E1" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F1" t="n">
-        <v>-11</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1</v>
+        <v>-0.046</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.007</v>
+        <v>-0.363</v>
       </c>
       <c r="C2" t="n">
-        <v>0.048</v>
+        <v>-0.414</v>
       </c>
       <c r="D2" t="n">
-        <v>101</v>
+        <v>-106</v>
       </c>
       <c r="E2" t="n">
-        <v>86</v>
+        <v>-14</v>
       </c>
       <c r="F2" t="n">
-        <v>172</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.173</v>
+        <v>0.202</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.044</v>
+        <v>0.11</v>
       </c>
       <c r="C3" t="n">
-        <v>0.229</v>
+        <v>-0.159</v>
       </c>
       <c r="D3" t="n">
-        <v>91</v>
+        <v>-95</v>
       </c>
       <c r="E3" t="n">
-        <v>-2</v>
+        <v>-68</v>
       </c>
       <c r="F3" t="n">
-        <v>-60</v>
+        <v>-139</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.157</v>
+        <v>0.134</v>
       </c>
       <c r="B4" t="n">
-        <v>0.024</v>
+        <v>0.126</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.208</v>
+        <v>0.377</v>
       </c>
       <c r="D4" t="n">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n">
-        <v>-26</v>
+        <v>17</v>
       </c>
       <c r="F4" t="n">
-        <v>-167</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.07199999999999999</v>
+        <v>0.673</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.184</v>
+        <v>-0.428</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2</v>
+        <v>0.285</v>
       </c>
       <c r="D5" t="n">
-        <v>-83</v>
+        <v>-162</v>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>-51</v>
       </c>
       <c r="F5" t="n">
-        <v>-169</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.161</v>
+        <v>0.171</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.061</v>
+        <v>-0.022</v>
       </c>
       <c r="C6" t="n">
-        <v>0.077</v>
+        <v>-0.66</v>
       </c>
       <c r="D6" t="n">
-        <v>-163</v>
+        <v>94</v>
       </c>
       <c r="E6" t="n">
-        <v>-25</v>
+        <v>-47</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.049</v>
+        <v>0.008</v>
       </c>
       <c r="B7" t="n">
-        <v>0.168</v>
+        <v>0.478</v>
       </c>
       <c r="C7" t="n">
-        <v>0.455</v>
+        <v>0.544</v>
       </c>
       <c r="D7" t="n">
-        <v>-155</v>
+        <v>-9</v>
       </c>
       <c r="E7" t="n">
-        <v>81</v>
+        <v>-22</v>
       </c>
       <c r="F7" t="n">
-        <v>-132</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.058</v>
+        <v>0.09</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.348</v>
+        <v>0.128</v>
       </c>
       <c r="C8" t="n">
-        <v>0.494</v>
+        <v>0.369</v>
       </c>
       <c r="D8" t="n">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
-        <v>24</v>
+        <v>-38</v>
       </c>
       <c r="F8" t="n">
-        <v>-49</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.326</v>
+        <v>0.304</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.076</v>
+        <v>-0.309</v>
       </c>
       <c r="C9" t="n">
-        <v>0.165</v>
+        <v>-0.37</v>
       </c>
       <c r="D9" t="n">
-        <v>-42</v>
+        <v>140</v>
       </c>
       <c r="E9" t="n">
-        <v>57</v>
+        <v>-27</v>
       </c>
       <c r="F9" t="n">
-        <v>-8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.124</v>
+        <v>0.344</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.08</v>
+        <v>0.093</v>
       </c>
       <c r="C10" t="n">
-        <v>0.242</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="D10" t="n">
+        <v>77</v>
+      </c>
+      <c r="E10" t="n">
         <v>18</v>
       </c>
-      <c r="E10" t="n">
-        <v>7</v>
-      </c>
       <c r="F10" t="n">
-        <v>-82</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed Q value max & min
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.028</v>
+        <v>-0.058</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.07099999999999999</v>
+        <v>-0.155</v>
       </c>
       <c r="C1" t="n">
-        <v>0.844</v>
+        <v>-0.156</v>
       </c>
       <c r="D1" t="n">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="E1" t="n">
-        <v>-6</v>
+        <v>-46</v>
       </c>
       <c r="F1" t="n">
-        <v>122</v>
+        <v>-110</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.046</v>
+        <v>-0.09</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.363</v>
+        <v>0.101</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.414</v>
+        <v>0.323</v>
       </c>
       <c r="D2" t="n">
-        <v>-106</v>
+        <v>43</v>
       </c>
       <c r="E2" t="n">
-        <v>-14</v>
+        <v>-45</v>
       </c>
       <c r="F2" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.202</v>
+        <v>-0.52</v>
       </c>
       <c r="B3" t="n">
-        <v>0.11</v>
+        <v>0.101</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.159</v>
+        <v>0.018</v>
       </c>
       <c r="D3" t="n">
-        <v>-95</v>
+        <v>158</v>
       </c>
       <c r="E3" t="n">
-        <v>-68</v>
+        <v>-38</v>
       </c>
       <c r="F3" t="n">
-        <v>-139</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.134</v>
+        <v>-0.134</v>
       </c>
       <c r="B4" t="n">
-        <v>0.126</v>
+        <v>0.13</v>
       </c>
       <c r="C4" t="n">
-        <v>0.377</v>
+        <v>0.051</v>
       </c>
       <c r="D4" t="n">
-        <v>22</v>
+        <v>-108</v>
       </c>
       <c r="E4" t="n">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.673</v>
+        <v>0.329</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.428</v>
+        <v>0.214</v>
       </c>
       <c r="C5" t="n">
-        <v>0.285</v>
+        <v>-0.233</v>
       </c>
       <c r="D5" t="n">
-        <v>-162</v>
+        <v>-42</v>
       </c>
       <c r="E5" t="n">
-        <v>-51</v>
+        <v>25</v>
       </c>
       <c r="F5" t="n">
-        <v>-126</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.171</v>
+        <v>0.059</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.022</v>
+        <v>-0.108</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.66</v>
+        <v>0.133</v>
       </c>
       <c r="D6" t="n">
-        <v>94</v>
+        <v>-107</v>
       </c>
       <c r="E6" t="n">
-        <v>-47</v>
+        <v>34</v>
       </c>
       <c r="F6" t="n">
-        <v>97</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.008</v>
+        <v>0.113</v>
       </c>
       <c r="B7" t="n">
-        <v>0.478</v>
+        <v>0.162</v>
       </c>
       <c r="C7" t="n">
-        <v>0.544</v>
+        <v>0.193</v>
       </c>
       <c r="D7" t="n">
-        <v>-9</v>
+        <v>106</v>
       </c>
       <c r="E7" t="n">
-        <v>-22</v>
+        <v>-42</v>
       </c>
       <c r="F7" t="n">
-        <v>-95</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.09</v>
+        <v>0.304</v>
       </c>
       <c r="B8" t="n">
-        <v>0.128</v>
+        <v>-0.126</v>
       </c>
       <c r="C8" t="n">
-        <v>0.369</v>
+        <v>0.412</v>
       </c>
       <c r="D8" t="n">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="E8" t="n">
-        <v>-38</v>
+        <v>-41</v>
       </c>
       <c r="F8" t="n">
-        <v>-171</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.304</v>
+        <v>0.168</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.309</v>
+        <v>-0.039</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.37</v>
+        <v>-0.207</v>
       </c>
       <c r="D9" t="n">
-        <v>140</v>
+        <v>-60</v>
       </c>
       <c r="E9" t="n">
-        <v>-27</v>
+        <v>36</v>
       </c>
       <c r="F9" t="n">
-        <v>56</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.344</v>
+        <v>0.234</v>
       </c>
       <c r="B10" t="n">
-        <v>0.093</v>
+        <v>0.027</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.532</v>
       </c>
       <c r="D10" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>-13</v>
       </c>
       <c r="F10" t="n">
-        <v>139</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add power cal & reward
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.058</v>
+        <v>0.11</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.155</v>
+        <v>0.211</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.156</v>
+        <v>-0.459</v>
       </c>
       <c r="D1" t="n">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E1" t="n">
-        <v>-46</v>
+        <v>29</v>
       </c>
       <c r="F1" t="n">
-        <v>-110</v>
+        <v>-86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.09</v>
+        <v>0.096</v>
       </c>
       <c r="B2" t="n">
-        <v>0.101</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.323</v>
+        <v>-0.002</v>
       </c>
       <c r="D2" t="n">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="E2" t="n">
-        <v>-45</v>
+        <v>-16</v>
       </c>
       <c r="F2" t="n">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.52</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>0.101</v>
+        <v>-0.139</v>
       </c>
       <c r="C3" t="n">
-        <v>0.018</v>
+        <v>0.463</v>
       </c>
       <c r="D3" t="n">
-        <v>158</v>
+        <v>-31</v>
       </c>
       <c r="E3" t="n">
-        <v>-38</v>
+        <v>46</v>
       </c>
       <c r="F3" t="n">
-        <v>-150</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.134</v>
+        <v>0.591</v>
       </c>
       <c r="B4" t="n">
-        <v>0.13</v>
+        <v>0.091</v>
       </c>
       <c r="C4" t="n">
-        <v>0.051</v>
+        <v>0.117</v>
       </c>
       <c r="D4" t="n">
-        <v>-108</v>
+        <v>144</v>
       </c>
       <c r="E4" t="n">
-        <v>56</v>
+        <v>-20</v>
       </c>
       <c r="F4" t="n">
-        <v>97</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.329</v>
+        <v>0.52</v>
       </c>
       <c r="B5" t="n">
-        <v>0.214</v>
+        <v>0.53</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.233</v>
+        <v>-0.049</v>
       </c>
       <c r="D5" t="n">
-        <v>-42</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F5" t="n">
-        <v>83</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.059</v>
+        <v>-0.146</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.108</v>
+        <v>-0.074</v>
       </c>
       <c r="C6" t="n">
-        <v>0.133</v>
+        <v>0.85</v>
       </c>
       <c r="D6" t="n">
-        <v>-107</v>
+        <v>-97</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>-4</v>
       </c>
       <c r="F6" t="n">
-        <v>-105</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.113</v>
+        <v>0.164</v>
       </c>
       <c r="B7" t="n">
-        <v>0.162</v>
+        <v>0.664</v>
       </c>
       <c r="C7" t="n">
-        <v>0.193</v>
+        <v>-0.191</v>
       </c>
       <c r="D7" t="n">
-        <v>106</v>
+        <v>-43</v>
       </c>
       <c r="E7" t="n">
-        <v>-42</v>
+        <v>54</v>
       </c>
       <c r="F7" t="n">
-        <v>173</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.304</v>
+        <v>0.247</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.126</v>
+        <v>-0.239</v>
       </c>
       <c r="C8" t="n">
-        <v>0.412</v>
+        <v>0.681</v>
       </c>
       <c r="D8" t="n">
-        <v>168</v>
+        <v>-173</v>
       </c>
       <c r="E8" t="n">
-        <v>-41</v>
+        <v>29</v>
       </c>
       <c r="F8" t="n">
-        <v>-30</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.168</v>
+        <v>-0.27</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.039</v>
+        <v>0.006</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.207</v>
+        <v>-0.42</v>
       </c>
       <c r="D9" t="n">
-        <v>-60</v>
+        <v>157</v>
       </c>
       <c r="E9" t="n">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F9" t="n">
-        <v>-78</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.234</v>
+        <v>-0.126</v>
       </c>
       <c r="B10" t="n">
-        <v>0.027</v>
+        <v>0.104</v>
       </c>
       <c r="C10" t="n">
-        <v>0.532</v>
+        <v>-0.216</v>
       </c>
       <c r="D10" t="n">
-        <v>89</v>
+        <v>-8</v>
       </c>
       <c r="E10" t="n">
-        <v>-13</v>
+        <v>9</v>
       </c>
       <c r="F10" t="n">
-        <v>-1</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add pybullet test code
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.11</v>
+        <v>0.655</v>
       </c>
       <c r="B1" t="n">
-        <v>0.211</v>
+        <v>0.24</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.459</v>
+        <v>-0.008</v>
       </c>
       <c r="D1" t="n">
-        <v>127</v>
+        <v>-105</v>
       </c>
       <c r="E1" t="n">
-        <v>29</v>
+        <v>-22</v>
       </c>
       <c r="F1" t="n">
-        <v>-86</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.096</v>
+        <v>0.194</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6929999999999999</v>
+        <v>-0.078</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.002</v>
+        <v>-0.541</v>
       </c>
       <c r="D2" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E2" t="n">
-        <v>-16</v>
+        <v>-36</v>
       </c>
       <c r="F2" t="n">
-        <v>103</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.07099999999999999</v>
+        <v>-0.544</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.139</v>
+        <v>-0.09</v>
       </c>
       <c r="C3" t="n">
-        <v>0.463</v>
+        <v>0.12</v>
       </c>
       <c r="D3" t="n">
-        <v>-31</v>
+        <v>131</v>
       </c>
       <c r="E3" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F3" t="n">
-        <v>113</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.591</v>
+        <v>-0.131</v>
       </c>
       <c r="B4" t="n">
-        <v>0.091</v>
+        <v>-0.006</v>
       </c>
       <c r="C4" t="n">
-        <v>0.117</v>
+        <v>-0.021</v>
       </c>
       <c r="D4" t="n">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="E4" t="n">
-        <v>-20</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>-95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.52</v>
+        <v>-0.433</v>
       </c>
       <c r="B5" t="n">
-        <v>0.53</v>
+        <v>-0.125</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.049</v>
+        <v>0.757</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>-29</v>
       </c>
       <c r="F5" t="n">
-        <v>148</v>
+        <v>-67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.146</v>
+        <v>-0.554</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.074</v>
+        <v>0.151</v>
       </c>
       <c r="C6" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="D6" t="n">
-        <v>-97</v>
+        <v>97</v>
       </c>
       <c r="E6" t="n">
-        <v>-4</v>
+        <v>61</v>
       </c>
       <c r="F6" t="n">
-        <v>-135</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.164</v>
+        <v>0.193</v>
       </c>
       <c r="B7" t="n">
-        <v>0.664</v>
+        <v>0.231</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.191</v>
+        <v>0.584</v>
       </c>
       <c r="D7" t="n">
-        <v>-43</v>
+        <v>-81</v>
       </c>
       <c r="E7" t="n">
-        <v>54</v>
+        <v>-9</v>
       </c>
       <c r="F7" t="n">
-        <v>-34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.247</v>
+        <v>0.339</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.239</v>
+        <v>0.203</v>
       </c>
       <c r="C8" t="n">
-        <v>0.681</v>
+        <v>-0.149</v>
       </c>
       <c r="D8" t="n">
-        <v>-173</v>
+        <v>-61</v>
       </c>
       <c r="E8" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" t="n">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.27</v>
+        <v>-0.268</v>
       </c>
       <c r="B9" t="n">
-        <v>0.006</v>
+        <v>-0.156</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.42</v>
+        <v>-0.211</v>
       </c>
       <c r="D9" t="n">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="E9" t="n">
-        <v>68</v>
+        <v>-28</v>
       </c>
       <c r="F9" t="n">
-        <v>-21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.126</v>
+        <v>-0.144</v>
       </c>
       <c r="B10" t="n">
-        <v>0.104</v>
+        <v>-0.355</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.216</v>
+        <v>-0.435</v>
       </c>
       <c r="D10" t="n">
-        <v>-8</v>
+        <v>-126</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F10" t="n">
-        <v>172</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add param for server train
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.655</v>
+        <v>-0.315</v>
       </c>
       <c r="B1" t="n">
-        <v>0.24</v>
+        <v>0.169</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.008</v>
+        <v>0.323</v>
       </c>
       <c r="D1" t="n">
-        <v>-105</v>
+        <v>16</v>
       </c>
       <c r="E1" t="n">
-        <v>-22</v>
+        <v>14</v>
       </c>
       <c r="F1" t="n">
-        <v>-100</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.194</v>
+        <v>-0.322</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.078</v>
+        <v>-0.014</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.541</v>
+        <v>0.032</v>
       </c>
       <c r="D2" t="n">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>-36</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.544</v>
+        <v>-0.297</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.09</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.12</v>
+        <v>0.045</v>
       </c>
       <c r="D3" t="n">
-        <v>131</v>
+        <v>-68</v>
       </c>
       <c r="E3" t="n">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F3" t="n">
-        <v>148</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.131</v>
+        <v>0.012</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.006</v>
+        <v>0.221</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.021</v>
+        <v>0.043</v>
       </c>
       <c r="D4" t="n">
-        <v>87</v>
+        <v>-87</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>-16</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>-106</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.433</v>
+        <v>0.178</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.125</v>
+        <v>0.118</v>
       </c>
       <c r="C5" t="n">
-        <v>0.757</v>
+        <v>0.055</v>
       </c>
       <c r="D5" t="n">
-        <v>16</v>
+        <v>-3</v>
       </c>
       <c r="E5" t="n">
-        <v>-29</v>
+        <v>-77</v>
       </c>
       <c r="F5" t="n">
-        <v>-67</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.554</v>
+        <v>0.236</v>
       </c>
       <c r="B6" t="n">
-        <v>0.151</v>
+        <v>0.179</v>
       </c>
       <c r="C6" t="n">
-        <v>0.14</v>
+        <v>0.355</v>
       </c>
       <c r="D6" t="n">
-        <v>97</v>
+        <v>-126</v>
       </c>
       <c r="E6" t="n">
-        <v>61</v>
+        <v>-15</v>
       </c>
       <c r="F6" t="n">
-        <v>-90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.193</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>0.231</v>
+        <v>-0.095</v>
       </c>
       <c r="C7" t="n">
-        <v>0.584</v>
+        <v>0.044</v>
       </c>
       <c r="D7" t="n">
-        <v>-81</v>
+        <v>38</v>
       </c>
       <c r="E7" t="n">
-        <v>-9</v>
+        <v>-43</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.339</v>
+        <v>0.106</v>
       </c>
       <c r="B8" t="n">
-        <v>0.203</v>
+        <v>-0.209</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.149</v>
+        <v>0.078</v>
       </c>
       <c r="D8" t="n">
-        <v>-61</v>
+        <v>68</v>
       </c>
       <c r="E8" t="n">
-        <v>33</v>
+        <v>-4</v>
       </c>
       <c r="F8" t="n">
-        <v>115</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.268</v>
+        <v>0.014</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.156</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.211</v>
+        <v>0.305</v>
       </c>
       <c r="D9" t="n">
-        <v>175</v>
+        <v>-176</v>
       </c>
       <c r="E9" t="n">
-        <v>-28</v>
+        <v>-29</v>
       </c>
       <c r="F9" t="n">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.144</v>
+        <v>-0.131</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.355</v>
+        <v>-0.237</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.435</v>
+        <v>0.525</v>
       </c>
       <c r="D10" t="n">
-        <v>-126</v>
+        <v>-73</v>
       </c>
       <c r="E10" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>106</v>
+        <v>-139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add power consumption train data
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.655</v>
+        <v>-0.244</v>
       </c>
       <c r="B1" t="n">
-        <v>0.24</v>
+        <v>0.053</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.008</v>
+        <v>0.554</v>
       </c>
       <c r="D1" t="n">
-        <v>-105</v>
+        <v>-170</v>
       </c>
       <c r="E1" t="n">
-        <v>-22</v>
+        <v>-10</v>
       </c>
       <c r="F1" t="n">
-        <v>-100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.194</v>
+        <v>-0.206</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.078</v>
+        <v>-0.368</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.541</v>
+        <v>-0.067</v>
       </c>
       <c r="D2" t="n">
         <v>97</v>
       </c>
       <c r="E2" t="n">
-        <v>-36</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.544</v>
+        <v>0.594</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.09</v>
+        <v>0.03</v>
       </c>
       <c r="C3" t="n">
-        <v>0.12</v>
+        <v>-0.209</v>
       </c>
       <c r="D3" t="n">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="E3" t="n">
-        <v>52</v>
+        <v>-25</v>
       </c>
       <c r="F3" t="n">
-        <v>148</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.131</v>
+        <v>-0.177</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.006</v>
+        <v>0.145</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.021</v>
+        <v>0.001</v>
       </c>
       <c r="D4" t="n">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>-176</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.433</v>
+        <v>0.476</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.125</v>
+        <v>0.203</v>
       </c>
       <c r="C5" t="n">
-        <v>0.757</v>
+        <v>-0.188</v>
       </c>
       <c r="D5" t="n">
-        <v>16</v>
+        <v>-179</v>
       </c>
       <c r="E5" t="n">
-        <v>-29</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>-67</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.554</v>
+        <v>-0.037</v>
       </c>
       <c r="B6" t="n">
-        <v>0.151</v>
+        <v>0.626</v>
       </c>
       <c r="C6" t="n">
-        <v>0.14</v>
+        <v>0.24</v>
       </c>
       <c r="D6" t="n">
-        <v>97</v>
+        <v>-23</v>
       </c>
       <c r="E6" t="n">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="F6" t="n">
-        <v>-90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.193</v>
+        <v>-0.081</v>
       </c>
       <c r="B7" t="n">
-        <v>0.231</v>
+        <v>0.199</v>
       </c>
       <c r="C7" t="n">
-        <v>0.584</v>
+        <v>-0.201</v>
       </c>
       <c r="D7" t="n">
-        <v>-81</v>
+        <v>95</v>
       </c>
       <c r="E7" t="n">
-        <v>-9</v>
+        <v>29</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.339</v>
+        <v>0.042</v>
       </c>
       <c r="B8" t="n">
-        <v>0.203</v>
+        <v>-0.083</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.149</v>
+        <v>0.06</v>
       </c>
       <c r="D8" t="n">
-        <v>-61</v>
+        <v>142</v>
       </c>
       <c r="E8" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>115</v>
+        <v>-164</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.268</v>
+        <v>0.054</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.156</v>
+        <v>-0.15</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.211</v>
+        <v>-0.095</v>
       </c>
       <c r="D9" t="n">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="E9" t="n">
-        <v>-28</v>
+        <v>-10</v>
       </c>
       <c r="F9" t="n">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.144</v>
+        <v>0.299</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.355</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.435</v>
+        <v>0.355</v>
       </c>
       <c r="D10" t="n">
-        <v>-126</v>
+        <v>54</v>
       </c>
       <c r="E10" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
server train tf agent error fixed
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.368</v>
+        <v>-0.097</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.348</v>
+        <v>-0.168</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.259</v>
+        <v>-0.138</v>
       </c>
       <c r="D1" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E1" t="n">
-        <v>-34</v>
+        <v>-46</v>
       </c>
       <c r="F1" t="n">
-        <v>172</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.03</v>
+        <v>-0.133</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.388</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.448</v>
+        <v>-0.081</v>
       </c>
       <c r="D2" t="n">
-        <v>-71</v>
+        <v>96</v>
       </c>
       <c r="E2" t="n">
-        <v>-30</v>
+        <v>-32</v>
       </c>
       <c r="F2" t="n">
-        <v>-116</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.034</v>
+        <v>0.031</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.261</v>
+        <v>-0.281</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.485</v>
+        <v>-0.159</v>
       </c>
       <c r="D3" t="n">
-        <v>172</v>
+        <v>-90</v>
       </c>
       <c r="E3" t="n">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="F3" t="n">
-        <v>38</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.118</v>
+        <v>-0.029</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.41</v>
+        <v>0.174</v>
       </c>
       <c r="C4" t="n">
-        <v>0.068</v>
+        <v>0.002</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>-91</v>
       </c>
       <c r="E4" t="n">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F4" t="n">
-        <v>88</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.375</v>
+        <v>0.068</v>
       </c>
       <c r="B5" t="n">
-        <v>0.239</v>
+        <v>-0.115</v>
       </c>
       <c r="C5" t="n">
-        <v>0.432</v>
+        <v>-0.193</v>
       </c>
       <c r="D5" t="n">
-        <v>-179</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F5" t="n">
-        <v>-60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.661</v>
+        <v>0.104</v>
       </c>
       <c r="B6" t="n">
-        <v>0.334</v>
+        <v>0.281</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.141</v>
+        <v>-0.392</v>
       </c>
       <c r="D6" t="n">
-        <v>168</v>
+        <v>-62</v>
       </c>
       <c r="E6" t="n">
-        <v>44</v>
+        <v>-18</v>
       </c>
       <c r="F6" t="n">
-        <v>53</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.125</v>
+        <v>-0.261</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.666</v>
+        <v>0.01</v>
       </c>
       <c r="C7" t="n">
-        <v>0.413</v>
+        <v>-0.108</v>
       </c>
       <c r="D7" t="n">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="E7" t="n">
-        <v>-9</v>
+        <v>45</v>
       </c>
       <c r="F7" t="n">
-        <v>-25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.027</v>
+        <v>0.077</v>
       </c>
       <c r="B8" t="n">
-        <v>0.176</v>
+        <v>-0.14</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.61</v>
+        <v>0.152</v>
       </c>
       <c r="D8" t="n">
-        <v>95</v>
+        <v>-64</v>
       </c>
       <c r="E8" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>-163</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.351</v>
+        <v>0.014</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.662</v>
+        <v>0.336</v>
       </c>
       <c r="C9" t="n">
-        <v>0.007</v>
+        <v>-0.041</v>
       </c>
       <c r="D9" t="n">
-        <v>97</v>
+        <v>-89</v>
       </c>
       <c r="E9" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F9" t="n">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.01</v>
+        <v>-0.143</v>
       </c>
       <c r="B10" t="n">
-        <v>0.107</v>
+        <v>-0.168</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.056</v>
+        <v>-0.141</v>
       </c>
       <c r="D10" t="n">
-        <v>83</v>
+        <v>-166</v>
       </c>
       <c r="E10" t="n">
-        <v>40</v>
+        <v>-19</v>
       </c>
       <c r="F10" t="n">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todo record episode step reward
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.5610000000000001</v>
+        <v>0.171</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.032</v>
+        <v>-0.117</v>
       </c>
       <c r="C1" t="n">
-        <v>0.526</v>
+        <v>-0.123</v>
       </c>
       <c r="D1" t="n">
-        <v>-89</v>
+        <v>-45</v>
       </c>
       <c r="E1" t="n">
-        <v>-60</v>
+        <v>10</v>
       </c>
       <c r="F1" t="n">
-        <v>-168</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.132</v>
+        <v>0.147</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.08699999999999999</v>
+        <v>0.413</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.025</v>
+        <v>0.184</v>
       </c>
       <c r="D2" t="n">
-        <v>-106</v>
+        <v>79</v>
       </c>
       <c r="E2" t="n">
-        <v>-31</v>
+        <v>30</v>
       </c>
       <c r="F2" t="n">
-        <v>-177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.468</v>
+        <v>-0.351</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.483</v>
+        <v>0.213</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.287</v>
+        <v>0.1</v>
       </c>
       <c r="D3" t="n">
-        <v>137</v>
+        <v>-111</v>
       </c>
       <c r="E3" t="n">
-        <v>47</v>
+        <v>-74</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.015</v>
+        <v>-0.304</v>
       </c>
       <c r="B4" t="n">
-        <v>0.444</v>
+        <v>-0.285</v>
       </c>
       <c r="C4" t="n">
-        <v>0.586</v>
+        <v>0.002</v>
       </c>
       <c r="D4" t="n">
-        <v>-40</v>
+        <v>152</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>-52</v>
       </c>
       <c r="F4" t="n">
-        <v>89</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.74</v>
+        <v>0.134</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.251</v>
+        <v>-0.163</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.053</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F5" t="n">
-        <v>-88</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.03</v>
+        <v>-0.186</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.07199999999999999</v>
+        <v>-0.615</v>
       </c>
       <c r="C6" t="n">
-        <v>1.075</v>
+        <v>0.289</v>
       </c>
       <c r="D6" t="n">
-        <v>-54</v>
+        <v>171</v>
       </c>
       <c r="E6" t="n">
-        <v>-45</v>
+        <v>46</v>
       </c>
       <c r="F6" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.217</v>
+        <v>-0.122</v>
       </c>
       <c r="B7" t="n">
-        <v>0.16</v>
+        <v>-0.055</v>
       </c>
       <c r="C7" t="n">
-        <v>0.15</v>
+        <v>0.016</v>
       </c>
       <c r="D7" t="n">
-        <v>-108</v>
+        <v>-141</v>
       </c>
       <c r="E7" t="n">
-        <v>-10</v>
+        <v>-24</v>
       </c>
       <c r="F7" t="n">
-        <v>18</v>
+        <v>-59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.314</v>
+        <v>-0.539</v>
       </c>
       <c r="B8" t="n">
-        <v>0.43</v>
+        <v>-0.038</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.53</v>
+        <v>0.356</v>
       </c>
       <c r="D8" t="n">
-        <v>80</v>
+        <v>-63</v>
       </c>
       <c r="E8" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" t="n">
-        <v>75</v>
+        <v>-176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.254</v>
+        <v>0.122</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.288</v>
+        <v>0.43</v>
       </c>
       <c r="C9" t="n">
-        <v>0.776</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>-85</v>
+        <v>54</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>-31</v>
       </c>
       <c r="F9" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.124</v>
+        <v>-0.316</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-0.303</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.215</v>
+        <v>-0.226</v>
       </c>
       <c r="D10" t="n">
-        <v>-40</v>
+        <v>-74</v>
       </c>
       <c r="E10" t="n">
-        <v>-38</v>
+        <v>-8</v>
       </c>
       <c r="F10" t="n">
-        <v>53</v>
+        <v>-156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added specified armlength & Test config motor
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.171</v>
+        <v>-0.354</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.117</v>
+        <v>-0.288</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.123</v>
+        <v>0.008</v>
       </c>
       <c r="D1" t="n">
-        <v>-45</v>
+        <v>-102</v>
       </c>
       <c r="E1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>-170</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.147</v>
+        <v>-0.301</v>
       </c>
       <c r="B2" t="n">
-        <v>0.413</v>
+        <v>0.108</v>
       </c>
       <c r="C2" t="n">
-        <v>0.184</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>79</v>
+        <v>-50</v>
       </c>
       <c r="E2" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
-        <v>96</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.351</v>
+        <v>-0.273</v>
       </c>
       <c r="B3" t="n">
-        <v>0.213</v>
+        <v>-0.268</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1</v>
+        <v>0.645</v>
       </c>
       <c r="D3" t="n">
-        <v>-111</v>
+        <v>121</v>
       </c>
       <c r="E3" t="n">
-        <v>-74</v>
+        <v>-70</v>
       </c>
       <c r="F3" t="n">
-        <v>-21</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.304</v>
+        <v>0.252</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.285</v>
+        <v>-0.29</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002</v>
+        <v>-0.139</v>
       </c>
       <c r="D4" t="n">
-        <v>152</v>
+        <v>-30</v>
       </c>
       <c r="E4" t="n">
-        <v>-52</v>
+        <v>-23</v>
       </c>
       <c r="F4" t="n">
-        <v>-171</v>
+        <v>-82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.134</v>
+        <v>0.237</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.163</v>
+        <v>0.068</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8129999999999999</v>
+        <v>-0.126</v>
       </c>
       <c r="D5" t="n">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>40</v>
+        <v>-33</v>
       </c>
       <c r="F5" t="n">
-        <v>-6</v>
+        <v>-162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.186</v>
+        <v>-0.014</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.615</v>
+        <v>0.154</v>
       </c>
       <c r="C6" t="n">
-        <v>0.289</v>
+        <v>-0.254</v>
       </c>
       <c r="D6" t="n">
-        <v>171</v>
+        <v>-55</v>
       </c>
       <c r="E6" t="n">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.122</v>
+        <v>-0.221</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.055</v>
+        <v>0.05</v>
       </c>
       <c r="C7" t="n">
-        <v>0.016</v>
+        <v>-0.333</v>
       </c>
       <c r="D7" t="n">
-        <v>-141</v>
+        <v>-17</v>
       </c>
       <c r="E7" t="n">
-        <v>-24</v>
+        <v>-80</v>
       </c>
       <c r="F7" t="n">
-        <v>-59</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.539</v>
+        <v>0.303</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.038</v>
+        <v>-0.153</v>
       </c>
       <c r="C8" t="n">
-        <v>0.356</v>
+        <v>0.188</v>
       </c>
       <c r="D8" t="n">
-        <v>-63</v>
+        <v>-81</v>
       </c>
       <c r="E8" t="n">
-        <v>53</v>
+        <v>-85</v>
       </c>
       <c r="F8" t="n">
-        <v>-176</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.122</v>
+        <v>0.384</v>
       </c>
       <c r="B9" t="n">
-        <v>0.43</v>
+        <v>0.194</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.316</v>
       </c>
       <c r="D9" t="n">
-        <v>54</v>
+        <v>-86</v>
       </c>
       <c r="E9" t="n">
-        <v>-31</v>
+        <v>-41</v>
       </c>
       <c r="F9" t="n">
-        <v>107</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.316</v>
+        <v>-0.131</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.303</v>
+        <v>0.18</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.226</v>
+        <v>-0.305</v>
       </c>
       <c r="D10" t="n">
-        <v>-74</v>
+        <v>-114</v>
       </c>
       <c r="E10" t="n">
-        <v>-8</v>
+        <v>22</v>
       </c>
       <c r="F10" t="n">
-        <v>-156</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add case 2 3,5dof actio & reset
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.806</v>
+        <v>-0.141</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.201</v>
+        <v>-0.08699999999999999</v>
       </c>
       <c r="C1" t="n">
-        <v>0.335</v>
+        <v>0.779</v>
       </c>
       <c r="D1" t="n">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="E1" t="n">
-        <v>-13</v>
+        <v>22</v>
       </c>
       <c r="F1" t="n">
-        <v>-83</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.122</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.265</v>
+        <v>-0.127</v>
       </c>
       <c r="C2" t="n">
-        <v>0.944</v>
+        <v>0.205</v>
       </c>
       <c r="D2" t="n">
-        <v>-16</v>
+        <v>-90</v>
       </c>
       <c r="E2" t="n">
-        <v>-43</v>
+        <v>-53</v>
       </c>
       <c r="F2" t="n">
-        <v>-4</v>
+        <v>-122</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.229</v>
+        <v>0.801</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.167</v>
+        <v>0.318</v>
       </c>
       <c r="C3" t="n">
-        <v>0.223</v>
+        <v>0.398</v>
       </c>
       <c r="D3" t="n">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="E3" t="n">
-        <v>-43</v>
+        <v>-23</v>
       </c>
       <c r="F3" t="n">
-        <v>143</v>
+        <v>-141</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.516</v>
+        <v>-0.205</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.744</v>
+        <v>-0.034</v>
       </c>
       <c r="C4" t="n">
-        <v>0.602</v>
+        <v>-0.755</v>
       </c>
       <c r="D4" t="n">
-        <v>-67</v>
+        <v>-133</v>
       </c>
       <c r="E4" t="n">
-        <v>-40</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>28</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.057</v>
+        <v>-0.239</v>
       </c>
       <c r="B5" t="n">
-        <v>0.637</v>
+        <v>-0.045</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.375</v>
+        <v>0.769</v>
       </c>
       <c r="D5" t="n">
-        <v>-97</v>
+        <v>-139</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>-121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.014</v>
+        <v>0.602</v>
       </c>
       <c r="B6" t="n">
-        <v>0.224</v>
+        <v>-0.353</v>
       </c>
       <c r="C6" t="n">
-        <v>1.121</v>
+        <v>-0.484</v>
       </c>
       <c r="D6" t="n">
-        <v>-149</v>
+        <v>162</v>
       </c>
       <c r="E6" t="n">
-        <v>-31</v>
+        <v>-20</v>
       </c>
       <c r="F6" t="n">
-        <v>132</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.661</v>
+        <v>0.405</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.156</v>
+        <v>0.143</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.393</v>
+        <v>0.166</v>
       </c>
       <c r="D7" t="n">
-        <v>127</v>
+        <v>-24</v>
       </c>
       <c r="E7" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>-62</v>
+        <v>-77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.227</v>
+        <v>-0.119</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.465</v>
+        <v>0.06</v>
       </c>
       <c r="C8" t="n">
-        <v>0.434</v>
+        <v>0.278</v>
       </c>
       <c r="D8" t="n">
-        <v>-27</v>
+        <v>-143</v>
       </c>
       <c r="E8" t="n">
-        <v>-66</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="n">
-        <v>-84</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.16</v>
+        <v>-0.209</v>
       </c>
       <c r="B9" t="n">
-        <v>0.186</v>
+        <v>0.032</v>
       </c>
       <c r="C9" t="n">
-        <v>1.031</v>
+        <v>1.071</v>
       </c>
       <c r="D9" t="n">
-        <v>-85</v>
+        <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>-36</v>
+        <v>63</v>
       </c>
       <c r="F9" t="n">
-        <v>-120</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.05</v>
+        <v>-0.376</v>
       </c>
       <c r="B10" t="n">
-        <v>0.626</v>
+        <v>0.273</v>
       </c>
       <c r="C10" t="n">
-        <v>0.343</v>
+        <v>0.922</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="E10" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="F10" t="n">
-        <v>39</v>
+        <v>-55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed model file location & case1 action fixed
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.141</v>
+        <v>-0.26</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-0.059</v>
       </c>
       <c r="C1" t="n">
-        <v>0.779</v>
+        <v>0.066</v>
       </c>
       <c r="D1" t="n">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E1" t="n">
-        <v>22</v>
+        <v>-65</v>
       </c>
       <c r="F1" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.122</v>
+        <v>-0.125</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.127</v>
+        <v>0.014</v>
       </c>
       <c r="C2" t="n">
-        <v>0.205</v>
+        <v>0.261</v>
       </c>
       <c r="D2" t="n">
-        <v>-90</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>-53</v>
+        <v>-4</v>
       </c>
       <c r="F2" t="n">
-        <v>-122</v>
+        <v>-159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.801</v>
+        <v>-0.206</v>
       </c>
       <c r="B3" t="n">
-        <v>0.318</v>
+        <v>-0.202</v>
       </c>
       <c r="C3" t="n">
-        <v>0.398</v>
+        <v>0.443</v>
       </c>
       <c r="D3" t="n">
-        <v>89</v>
+        <v>-44</v>
       </c>
       <c r="E3" t="n">
-        <v>-23</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>-141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.205</v>
+        <v>-0.196</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.034</v>
+        <v>-0.248</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.755</v>
+        <v>0.418</v>
       </c>
       <c r="D4" t="n">
-        <v>-133</v>
+        <v>89</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F4" t="n">
-        <v>121</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.239</v>
+        <v>-0.125</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.045</v>
+        <v>-0.116</v>
       </c>
       <c r="C5" t="n">
-        <v>0.769</v>
+        <v>0.074</v>
       </c>
       <c r="D5" t="n">
-        <v>-139</v>
+        <v>-88</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="F5" t="n">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.602</v>
+        <v>-0.013</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.353</v>
+        <v>-0.08699999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.484</v>
+        <v>0.18</v>
       </c>
       <c r="D6" t="n">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="E6" t="n">
-        <v>-20</v>
+        <v>41</v>
       </c>
       <c r="F6" t="n">
-        <v>94</v>
+        <v>-83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.405</v>
+        <v>0.277</v>
       </c>
       <c r="B7" t="n">
-        <v>0.143</v>
+        <v>0.12</v>
       </c>
       <c r="C7" t="n">
-        <v>0.166</v>
+        <v>0.514</v>
       </c>
       <c r="D7" t="n">
-        <v>-24</v>
+        <v>-143</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>-9</v>
       </c>
       <c r="F7" t="n">
-        <v>-77</v>
+        <v>-92</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.119</v>
+        <v>0.022</v>
       </c>
       <c r="B8" t="n">
-        <v>0.06</v>
+        <v>-0.058</v>
       </c>
       <c r="C8" t="n">
-        <v>0.278</v>
+        <v>0.055</v>
       </c>
       <c r="D8" t="n">
-        <v>-143</v>
+        <v>125</v>
       </c>
       <c r="E8" t="n">
-        <v>-14</v>
+        <v>-37</v>
       </c>
       <c r="F8" t="n">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.209</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="B9" t="n">
-        <v>0.032</v>
+        <v>0.156</v>
       </c>
       <c r="C9" t="n">
-        <v>1.071</v>
+        <v>0.209</v>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E9" t="n">
-        <v>63</v>
+        <v>-59</v>
       </c>
       <c r="F9" t="n">
-        <v>-134</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.376</v>
+        <v>-0.417</v>
       </c>
       <c r="B10" t="n">
-        <v>0.273</v>
+        <v>-0.094</v>
       </c>
       <c r="C10" t="n">
-        <v>0.922</v>
+        <v>0.366</v>
       </c>
       <c r="D10" t="n">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E10" t="n">
-        <v>37</v>
+        <v>-9</v>
       </c>
       <c r="F10" t="n">
-        <v>-55</v>
+        <v>-99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
case2 train fixed arm length
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.806</v>
+        <v>0.45</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.201</v>
+        <v>0.266</v>
       </c>
       <c r="C1" t="n">
-        <v>0.335</v>
+        <v>-0.508</v>
       </c>
       <c r="D1" t="n">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E1" t="n">
-        <v>-13</v>
+        <v>47</v>
       </c>
       <c r="F1" t="n">
-        <v>-83</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.06</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.265</v>
+        <v>0.404</v>
       </c>
       <c r="C2" t="n">
-        <v>0.944</v>
+        <v>-0.304</v>
       </c>
       <c r="D2" t="n">
-        <v>-16</v>
+        <v>-178</v>
       </c>
       <c r="E2" t="n">
-        <v>-43</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>-4</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.229</v>
+        <v>-0.076</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.167</v>
+        <v>-0.138</v>
       </c>
       <c r="C3" t="n">
-        <v>0.223</v>
+        <v>0.173</v>
       </c>
       <c r="D3" t="n">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v>-43</v>
+        <v>74</v>
       </c>
       <c r="F3" t="n">
-        <v>143</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.516</v>
+        <v>0.033</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.744</v>
+        <v>-0.114</v>
       </c>
       <c r="C4" t="n">
-        <v>0.602</v>
+        <v>-0.482</v>
       </c>
       <c r="D4" t="n">
-        <v>-67</v>
+        <v>-51</v>
       </c>
       <c r="E4" t="n">
-        <v>-40</v>
+        <v>31</v>
       </c>
       <c r="F4" t="n">
-        <v>28</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.057</v>
+        <v>0.164</v>
       </c>
       <c r="B5" t="n">
-        <v>0.637</v>
+        <v>0.078</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.375</v>
+        <v>0.163</v>
       </c>
       <c r="D5" t="n">
-        <v>-97</v>
+        <v>-179</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F5" t="n">
-        <v>-121</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.014</v>
+        <v>-0.116</v>
       </c>
       <c r="B6" t="n">
-        <v>0.224</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>1.121</v>
+        <v>-0.288</v>
       </c>
       <c r="D6" t="n">
-        <v>-149</v>
+        <v>-12</v>
       </c>
       <c r="E6" t="n">
-        <v>-31</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.661</v>
+        <v>-0.343</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.156</v>
+        <v>-0.052</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.393</v>
+        <v>0.511</v>
       </c>
       <c r="D7" t="n">
-        <v>127</v>
+        <v>-175</v>
       </c>
       <c r="E7" t="n">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F7" t="n">
-        <v>-62</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.227</v>
+        <v>-0.079</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.465</v>
+        <v>0.334</v>
       </c>
       <c r="C8" t="n">
-        <v>0.434</v>
+        <v>0.028</v>
       </c>
       <c r="D8" t="n">
-        <v>-27</v>
+        <v>42</v>
       </c>
       <c r="E8" t="n">
-        <v>-66</v>
+        <v>31</v>
       </c>
       <c r="F8" t="n">
-        <v>-84</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.16</v>
+        <v>-0.121</v>
       </c>
       <c r="B9" t="n">
-        <v>0.186</v>
+        <v>-0.307</v>
       </c>
       <c r="C9" t="n">
-        <v>1.031</v>
+        <v>-0.285</v>
       </c>
       <c r="D9" t="n">
-        <v>-85</v>
+        <v>-29</v>
       </c>
       <c r="E9" t="n">
-        <v>-36</v>
+        <v>-60</v>
       </c>
       <c r="F9" t="n">
-        <v>-120</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.05</v>
+        <v>-0.384</v>
       </c>
       <c r="B10" t="n">
-        <v>0.626</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>0.343</v>
+        <v>0.701</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E10" t="n">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="F10" t="n">
-        <v>39</v>
+        <v>-105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed & test model
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.26</v>
+        <v>-0.053</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.059</v>
+        <v>0.414</v>
       </c>
       <c r="C1" t="n">
-        <v>0.066</v>
+        <v>1.124</v>
       </c>
       <c r="D1" t="n">
-        <v>89</v>
+        <v>-33</v>
       </c>
       <c r="E1" t="n">
-        <v>-65</v>
+        <v>37</v>
       </c>
       <c r="F1" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.125</v>
+        <v>-0.119</v>
       </c>
       <c r="B2" t="n">
-        <v>0.014</v>
+        <v>0.09</v>
       </c>
       <c r="C2" t="n">
-        <v>0.261</v>
+        <v>0.089</v>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>-90</v>
       </c>
       <c r="E2" t="n">
-        <v>-4</v>
+        <v>-68</v>
       </c>
       <c r="F2" t="n">
-        <v>-159</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.206</v>
+        <v>-0.201</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.202</v>
+        <v>0.099</v>
       </c>
       <c r="C3" t="n">
-        <v>0.443</v>
+        <v>-0.644</v>
       </c>
       <c r="D3" t="n">
-        <v>-44</v>
+        <v>-25</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="F3" t="n">
-        <v>157</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.196</v>
+        <v>-0.521</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.248</v>
+        <v>-0.095</v>
       </c>
       <c r="C4" t="n">
-        <v>0.418</v>
+        <v>0.976</v>
       </c>
       <c r="D4" t="n">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.125</v>
+        <v>0.145</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.116</v>
+        <v>0.163</v>
       </c>
       <c r="C5" t="n">
-        <v>0.074</v>
+        <v>-0.84</v>
       </c>
       <c r="D5" t="n">
-        <v>-88</v>
+        <v>94</v>
       </c>
       <c r="E5" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F5" t="n">
-        <v>140</v>
+        <v>-175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.013</v>
+        <v>0.027</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-0.168</v>
       </c>
       <c r="C6" t="n">
-        <v>0.18</v>
+        <v>-0.511</v>
       </c>
       <c r="D6" t="n">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="E6" t="n">
-        <v>41</v>
+        <v>-13</v>
       </c>
       <c r="F6" t="n">
-        <v>-83</v>
+        <v>-122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.277</v>
+        <v>0.157</v>
       </c>
       <c r="B7" t="n">
-        <v>0.12</v>
+        <v>0.668</v>
       </c>
       <c r="C7" t="n">
-        <v>0.514</v>
+        <v>-0.052</v>
       </c>
       <c r="D7" t="n">
-        <v>-143</v>
+        <v>-84</v>
       </c>
       <c r="E7" t="n">
-        <v>-9</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
-        <v>-92</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.022</v>
+        <v>-0.954</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.058</v>
+        <v>0.062</v>
       </c>
       <c r="C8" t="n">
-        <v>0.055</v>
+        <v>-0.051</v>
       </c>
       <c r="D8" t="n">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="E8" t="n">
-        <v>-37</v>
+        <v>51</v>
       </c>
       <c r="F8" t="n">
-        <v>146</v>
+        <v>-161</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.404</v>
       </c>
       <c r="B9" t="n">
-        <v>0.156</v>
+        <v>0.388</v>
       </c>
       <c r="C9" t="n">
-        <v>0.209</v>
+        <v>-0.5669999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-59</v>
+        <v>17</v>
       </c>
       <c r="F9" t="n">
-        <v>134</v>
+        <v>-173</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.417</v>
+        <v>0.459</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.094</v>
+        <v>-0.616</v>
       </c>
       <c r="C10" t="n">
-        <v>0.366</v>
+        <v>0.576</v>
       </c>
       <c r="D10" t="n">
-        <v>63</v>
+        <v>-89</v>
       </c>
       <c r="E10" t="n">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="F10" t="n">
-        <v>-99</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed no add payload set
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.053</v>
+        <v>-0.004</v>
       </c>
       <c r="B1" t="n">
-        <v>0.414</v>
+        <v>-0.672</v>
       </c>
       <c r="C1" t="n">
-        <v>1.124</v>
+        <v>-0.433</v>
       </c>
       <c r="D1" t="n">
-        <v>-33</v>
+        <v>-65</v>
       </c>
       <c r="E1" t="n">
-        <v>37</v>
+        <v>-18</v>
       </c>
       <c r="F1" t="n">
-        <v>55</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.119</v>
+        <v>0.171</v>
       </c>
       <c r="B2" t="n">
-        <v>0.09</v>
+        <v>0.13</v>
       </c>
       <c r="C2" t="n">
-        <v>0.089</v>
+        <v>-0.307</v>
       </c>
       <c r="D2" t="n">
-        <v>-90</v>
+        <v>-115</v>
       </c>
       <c r="E2" t="n">
-        <v>-68</v>
+        <v>44</v>
       </c>
       <c r="F2" t="n">
-        <v>12</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.201</v>
+        <v>-0.323</v>
       </c>
       <c r="B3" t="n">
-        <v>0.099</v>
+        <v>0.167</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.644</v>
+        <v>-0.212</v>
       </c>
       <c r="D3" t="n">
-        <v>-25</v>
+        <v>-22</v>
       </c>
       <c r="E3" t="n">
-        <v>-6</v>
+        <v>-46</v>
       </c>
       <c r="F3" t="n">
-        <v>126</v>
+        <v>-82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.521</v>
+        <v>0.475</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.095</v>
+        <v>-0.104</v>
       </c>
       <c r="C4" t="n">
-        <v>0.976</v>
+        <v>-0.651</v>
       </c>
       <c r="D4" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="F4" t="n">
-        <v>52</v>
+        <v>-112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.145</v>
+        <v>0.217</v>
       </c>
       <c r="B5" t="n">
-        <v>0.163</v>
+        <v>0.255</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.84</v>
+        <v>1.019</v>
       </c>
       <c r="D5" t="n">
-        <v>94</v>
+        <v>-57</v>
       </c>
       <c r="E5" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" t="n">
-        <v>-175</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.027</v>
+        <v>-0.199</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.168</v>
+        <v>0.08</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.511</v>
+        <v>0.4</v>
       </c>
       <c r="D6" t="n">
-        <v>163</v>
+        <v>-164</v>
       </c>
       <c r="E6" t="n">
-        <v>-13</v>
+        <v>68</v>
       </c>
       <c r="F6" t="n">
-        <v>-122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.157</v>
+        <v>-0.122</v>
       </c>
       <c r="B7" t="n">
-        <v>0.668</v>
+        <v>1.004</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.052</v>
+        <v>0.032</v>
       </c>
       <c r="D7" t="n">
-        <v>-84</v>
+        <v>-91</v>
       </c>
       <c r="E7" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>-95</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.954</v>
+        <v>-0.484</v>
       </c>
       <c r="B8" t="n">
-        <v>0.062</v>
+        <v>0.619</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.051</v>
+        <v>0.894</v>
       </c>
       <c r="D8" t="n">
-        <v>59</v>
+        <v>-126</v>
       </c>
       <c r="E8" t="n">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F8" t="n">
-        <v>-161</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.404</v>
+        <v>0.628</v>
       </c>
       <c r="B9" t="n">
-        <v>0.388</v>
+        <v>0.285</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.5669999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="E9" t="n">
-        <v>17</v>
+        <v>-38</v>
       </c>
       <c r="F9" t="n">
-        <v>-173</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.459</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.616</v>
+        <v>-0.654</v>
       </c>
       <c r="C10" t="n">
-        <v>0.576</v>
+        <v>-0.33</v>
       </c>
       <c r="D10" t="n">
-        <v>-89</v>
+        <v>84</v>
       </c>
       <c r="E10" t="n">
         <v>11</v>
       </c>
       <c r="F10" t="n">
-        <v>129</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test point c
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.063</v>
+        <v>-0.12</v>
       </c>
       <c r="B1" t="n">
-        <v>0.2</v>
+        <v>0.147</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.434</v>
+        <v>-0.201</v>
       </c>
       <c r="D1" t="n">
-        <v>-123</v>
+        <v>91</v>
       </c>
       <c r="E1" t="n">
-        <v>-27</v>
+        <v>28</v>
       </c>
       <c r="F1" t="n">
-        <v>64</v>
+        <v>-160</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.342</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.223</v>
+        <v>-0.295</v>
       </c>
       <c r="C2" t="n">
-        <v>0.647</v>
+        <v>0.461</v>
       </c>
       <c r="D2" t="n">
-        <v>-17</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>-54</v>
       </c>
       <c r="F2" t="n">
-        <v>-29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.026</v>
+        <v>-0.191</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.284</v>
+        <v>-0.205</v>
       </c>
       <c r="C3" t="n">
-        <v>0.049</v>
+        <v>0.617</v>
       </c>
       <c r="D3" t="n">
-        <v>-101</v>
+        <v>-157</v>
       </c>
       <c r="E3" t="n">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>97</v>
+        <v>-114</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.538</v>
+        <v>-0.154</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.526</v>
+        <v>0.259</v>
       </c>
       <c r="C4" t="n">
-        <v>0.916</v>
+        <v>0.615</v>
       </c>
       <c r="D4" t="n">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E4" t="n">
-        <v>-12</v>
+        <v>39</v>
       </c>
       <c r="F4" t="n">
-        <v>55</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.184</v>
+        <v>0.165</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.132</v>
+        <v>-0.059</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.101</v>
+        <v>0.846</v>
       </c>
       <c r="D5" t="n">
-        <v>-71</v>
+        <v>-3</v>
       </c>
       <c r="E5" t="n">
-        <v>-44</v>
+        <v>-11</v>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>-92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.037</v>
+        <v>0.108</v>
       </c>
       <c r="B6" t="n">
-        <v>0.055</v>
+        <v>-0.165</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.713</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>-37</v>
+        <v>113</v>
       </c>
       <c r="E6" t="n">
-        <v>48</v>
+        <v>-3</v>
       </c>
       <c r="F6" t="n">
-        <v>-119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.056</v>
+        <v>-0.492</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.427</v>
+        <v>0.095</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="D7" t="n">
-        <v>-77</v>
+        <v>-89</v>
       </c>
       <c r="E7" t="n">
-        <v>-37</v>
+        <v>-19</v>
       </c>
       <c r="F7" t="n">
-        <v>42</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.141</v>
+        <v>-0.1</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.012</v>
+        <v>0.485</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.797</v>
+        <v>0.734</v>
       </c>
       <c r="D8" t="n">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="E8" t="n">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>39</v>
+        <v>-152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.474</v>
+        <v>0.046</v>
       </c>
       <c r="B9" t="n">
-        <v>0.278</v>
+        <v>-0.309</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.701</v>
+        <v>0.168</v>
       </c>
       <c r="D9" t="n">
-        <v>-133</v>
+        <v>-32</v>
       </c>
       <c r="E9" t="n">
-        <v>-52</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>-165</v>
+        <v>-71</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.33</v>
+        <v>-0.278</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.302</v>
+        <v>-0.252</v>
       </c>
       <c r="C10" t="n">
-        <v>0.877</v>
+        <v>0.634</v>
       </c>
       <c r="D10" t="n">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="E10" t="n">
-        <v>-67</v>
+        <v>54</v>
       </c>
       <c r="F10" t="n">
-        <v>-85</v>
+        <v>-19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add original test case1
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,139 +423,139 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.12</v>
+        <v>0.187</v>
       </c>
       <c r="B1" t="n">
-        <v>0.147</v>
+        <v>0.058</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.201</v>
+        <v>-0.231</v>
       </c>
       <c r="D1" t="n">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="E1" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F1" t="n">
-        <v>-160</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.206</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.295</v>
+        <v>-0.08799999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.461</v>
+        <v>0.408</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>-168</v>
       </c>
       <c r="E2" t="n">
-        <v>-54</v>
+        <v>-44</v>
       </c>
       <c r="F2" t="n">
-        <v>49</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.191</v>
+        <v>0.467</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.205</v>
+        <v>0.118</v>
       </c>
       <c r="C3" t="n">
-        <v>0.617</v>
+        <v>0.616</v>
       </c>
       <c r="D3" t="n">
-        <v>-157</v>
+        <v>-152</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="F3" t="n">
-        <v>-114</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.154</v>
+        <v>-0.046</v>
       </c>
       <c r="B4" t="n">
-        <v>0.259</v>
+        <v>0.033</v>
       </c>
       <c r="C4" t="n">
-        <v>0.615</v>
+        <v>0.533</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>-38</v>
       </c>
       <c r="E4" t="n">
-        <v>39</v>
+        <v>-35</v>
       </c>
       <c r="F4" t="n">
-        <v>-75</v>
+        <v>-127</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.165</v>
+        <v>-0.294</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.059</v>
+        <v>0.099</v>
       </c>
       <c r="C5" t="n">
-        <v>0.846</v>
+        <v>0.292</v>
       </c>
       <c r="D5" t="n">
-        <v>-3</v>
+        <v>-74</v>
       </c>
       <c r="E5" t="n">
-        <v>-11</v>
+        <v>47</v>
       </c>
       <c r="F5" t="n">
-        <v>-92</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.108</v>
+        <v>0.094</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.165</v>
+        <v>-0.107</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5679999999999999</v>
+        <v>0.228</v>
       </c>
       <c r="D6" t="n">
         <v>113</v>
       </c>
       <c r="E6" t="n">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.492</v>
+        <v>0.317</v>
       </c>
       <c r="B7" t="n">
-        <v>0.095</v>
+        <v>0.183</v>
       </c>
       <c r="C7" t="n">
-        <v>0.36</v>
+        <v>0.082</v>
       </c>
       <c r="D7" t="n">
-        <v>-89</v>
+        <v>177</v>
       </c>
       <c r="E7" t="n">
-        <v>-19</v>
+        <v>67</v>
       </c>
       <c r="F7" t="n">
         <v>149</v>
@@ -563,62 +563,62 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.1</v>
+        <v>0.308</v>
       </c>
       <c r="B8" t="n">
-        <v>0.485</v>
+        <v>0.348</v>
       </c>
       <c r="C8" t="n">
-        <v>0.734</v>
+        <v>0.095</v>
       </c>
       <c r="D8" t="n">
-        <v>86</v>
+        <v>-100</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F8" t="n">
-        <v>-152</v>
+        <v>-106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.046</v>
+        <v>-0.094</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.309</v>
+        <v>-0.286</v>
       </c>
       <c r="C9" t="n">
-        <v>0.168</v>
+        <v>0.441</v>
       </c>
       <c r="D9" t="n">
-        <v>-32</v>
+        <v>128</v>
       </c>
       <c r="E9" t="n">
         <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>-71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.278</v>
+        <v>0.078</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.252</v>
+        <v>-0.541</v>
       </c>
       <c r="C10" t="n">
-        <v>0.634</v>
+        <v>0.233</v>
       </c>
       <c r="D10" t="n">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="E10" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F10" t="n">
-        <v>-19</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add single_arm v19 test fix urdf fail
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.187</v>
+        <v>-0.047</v>
       </c>
       <c r="B1" t="n">
-        <v>0.058</v>
+        <v>0.026</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.231</v>
+        <v>0.522</v>
       </c>
       <c r="D1" t="n">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="E1" t="n">
-        <v>35</v>
+        <v>-33</v>
       </c>
       <c r="F1" t="n">
-        <v>-44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.206</v>
+        <v>-0.479</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.08799999999999999</v>
+        <v>-0.141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.408</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>-168</v>
+        <v>46</v>
       </c>
       <c r="E2" t="n">
-        <v>-44</v>
+        <v>-62</v>
       </c>
       <c r="F2" t="n">
-        <v>-56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.467</v>
+        <v>-0.062</v>
       </c>
       <c r="B3" t="n">
-        <v>0.118</v>
+        <v>-0.307</v>
       </c>
       <c r="C3" t="n">
-        <v>0.616</v>
+        <v>0.759</v>
       </c>
       <c r="D3" t="n">
-        <v>-152</v>
+        <v>110</v>
       </c>
       <c r="E3" t="n">
-        <v>68</v>
+        <v>-11</v>
       </c>
       <c r="F3" t="n">
-        <v>-55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.046</v>
+        <v>0.043</v>
       </c>
       <c r="B4" t="n">
-        <v>0.033</v>
+        <v>0.153</v>
       </c>
       <c r="C4" t="n">
-        <v>0.533</v>
+        <v>0.496</v>
       </c>
       <c r="D4" t="n">
-        <v>-38</v>
+        <v>107</v>
       </c>
       <c r="E4" t="n">
-        <v>-35</v>
+        <v>74</v>
       </c>
       <c r="F4" t="n">
-        <v>-127</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.294</v>
+        <v>0.092</v>
       </c>
       <c r="B5" t="n">
-        <v>0.099</v>
+        <v>0.008</v>
       </c>
       <c r="C5" t="n">
-        <v>0.292</v>
+        <v>0.281</v>
       </c>
       <c r="D5" t="n">
-        <v>-74</v>
+        <v>126</v>
       </c>
       <c r="E5" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-63</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.094</v>
+        <v>0.378</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.107</v>
+        <v>0.208</v>
       </c>
       <c r="C6" t="n">
-        <v>0.228</v>
+        <v>0.611</v>
       </c>
       <c r="D6" t="n">
-        <v>113</v>
+        <v>-32</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>76</v>
       </c>
       <c r="F6" t="n">
-        <v>-40</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.317</v>
+        <v>-0.523</v>
       </c>
       <c r="B7" t="n">
-        <v>0.183</v>
+        <v>0.197</v>
       </c>
       <c r="C7" t="n">
-        <v>0.082</v>
+        <v>-0</v>
       </c>
       <c r="D7" t="n">
-        <v>177</v>
+        <v>-150</v>
       </c>
       <c r="E7" t="n">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F7" t="n">
-        <v>149</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.308</v>
+        <v>-0.354</v>
       </c>
       <c r="B8" t="n">
-        <v>0.348</v>
+        <v>-0.251</v>
       </c>
       <c r="C8" t="n">
-        <v>0.095</v>
+        <v>0.614</v>
       </c>
       <c r="D8" t="n">
-        <v>-100</v>
+        <v>69</v>
       </c>
       <c r="E8" t="n">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="F8" t="n">
-        <v>-106</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.094</v>
+        <v>-0.223</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.286</v>
+        <v>0.194</v>
       </c>
       <c r="C9" t="n">
-        <v>0.441</v>
+        <v>0.067</v>
       </c>
       <c r="D9" t="n">
-        <v>128</v>
+        <v>-50</v>
       </c>
       <c r="E9" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.078</v>
+        <v>-0.285</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.541</v>
+        <v>-0.168</v>
       </c>
       <c r="C10" t="n">
-        <v>0.233</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>103</v>
+        <v>-60</v>
       </c>
       <c r="E10" t="n">
-        <v>59</v>
+        <v>-13</v>
       </c>
       <c r="F10" t="n">
-        <v>91</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>